<commit_message>
loading and notfound files
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD786C9-F430-4FAF-AF6C-397C3CD4337C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF71AED-39DE-46A3-A29F-BF81C6538BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F4D59D-8EC0-4300-B06F-D1EA277B0BF1}">
   <dimension ref="A1:R73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1003,11 +1003,11 @@
       <c r="J2" s="23"/>
       <c r="K2" s="19">
         <f>(K4+(L4/60))/60</f>
-        <v>1.1244444444444446</v>
+        <v>1.3583333333333334</v>
       </c>
       <c r="L2" s="18">
         <f>(K4+(L4/60))</f>
-        <v>67.466666666666669</v>
+        <v>81.5</v>
       </c>
       <c r="M2" s="21"/>
       <c r="N2" s="21"/>
@@ -1089,11 +1089,11 @@
       </c>
       <c r="K4" s="14">
         <f>SUM(K5:K72)</f>
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="L4" s="14">
         <f>SUM(L5:L72)</f>
-        <v>508</v>
+        <v>630</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>0</v>
@@ -2138,9 +2138,15 @@
       <c r="I25" s="10">
         <v>4.3749999999999997E-2</v>
       </c>
-      <c r="J25" s="11"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="13"/>
+      <c r="J25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="12">
+        <v>3</v>
+      </c>
+      <c r="L25" s="13">
+        <v>59</v>
+      </c>
       <c r="M25" s="9">
         <v>45358</v>
       </c>
@@ -2182,9 +2188,15 @@
       <c r="I26" s="10">
         <v>4.5833333333333399E-2</v>
       </c>
-      <c r="J26" s="11"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="13"/>
+      <c r="J26" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" s="12">
+        <v>2</v>
+      </c>
+      <c r="L26" s="13">
+        <v>54</v>
+      </c>
       <c r="M26" s="9">
         <v>45359</v>
       </c>
@@ -2226,9 +2238,15 @@
       <c r="I27" s="10">
         <v>4.7916666666666698E-2</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="13"/>
+      <c r="J27" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="12">
+        <v>7</v>
+      </c>
+      <c r="L27" s="13">
+        <v>9</v>
+      </c>
       <c r="M27" s="9">
         <v>45360</v>
       </c>

</xml_diff>

<commit_message>
Creating Api For issues
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mosta\OneDrive\Desktop\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7158E83-7E71-4F2E-97F2-78C91303C60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EFEFA2-212E-4012-87A6-C759316155EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -910,7 +910,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -974,11 +974,11 @@
       <c r="D2" s="20"/>
       <c r="E2" s="18">
         <f>(E3+(F3/60))/60</f>
-        <v>0.60583333333333333</v>
+        <v>0.72083333333333333</v>
       </c>
       <c r="F2" s="19">
         <f>(E3+(F3/60))</f>
-        <v>36.35</v>
+        <v>43.25</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
@@ -1020,11 +1020,11 @@
       </c>
       <c r="E3" s="12">
         <f>SUM(E4:E71)</f>
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F3" s="12">
         <f>SUM(F4:F71)</f>
-        <v>441</v>
+        <v>495</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="M4" s="8">
         <f ca="1">TODAY()</f>
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="N4" s="9">
         <v>0</v>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="M5" s="8">
         <f ca="1">M4+1</f>
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="N5" s="9">
         <v>1.0416666666666667E-3</v>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="M6" s="8">
         <f t="shared" ref="M6:M61" ca="1" si="1">M5+1</f>
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="N6" s="9">
         <v>2.0833333333333298E-3</v>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="M7" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="N7" s="9">
         <v>3.1250000000000002E-3</v>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="M8" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="N8" s="9">
         <v>4.1666666666666701E-3</v>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="M9" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="N9" s="9">
         <v>5.2083333333333296E-3</v>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="M10" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="N10" s="9">
         <v>6.2500000000000003E-3</v>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="M11" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45379</v>
+        <v>45380</v>
       </c>
       <c r="N11" s="9">
         <v>7.2916666666666703E-3</v>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="M12" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45380</v>
+        <v>45381</v>
       </c>
       <c r="N12" s="9">
         <v>8.3333333333333297E-3</v>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="M13" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45381</v>
+        <v>45382</v>
       </c>
       <c r="N13" s="9">
         <v>9.3749999999999997E-3</v>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="M14" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45382</v>
+        <v>45383</v>
       </c>
       <c r="N14" s="9">
         <v>1.0416666666666701E-2</v>
@@ -1678,7 +1678,7 @@
       </c>
       <c r="M15" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45383</v>
+        <v>45384</v>
       </c>
       <c r="N15" s="9">
         <v>1.14583333333333E-2</v>
@@ -1701,9 +1701,15 @@
       <c r="C16" s="9">
         <v>1.35416666666667E-2</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="D16" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="11">
+        <v>6</v>
+      </c>
+      <c r="F16" s="11">
+        <v>54</v>
+      </c>
       <c r="G16" s="8">
         <v>45343</v>
       </c>
@@ -1724,7 +1730,7 @@
       </c>
       <c r="M16" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45384</v>
+        <v>45385</v>
       </c>
       <c r="N16" s="9">
         <v>1.2500000000000001E-2</v>
@@ -1770,7 +1776,7 @@
       </c>
       <c r="M17" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45385</v>
+        <v>45386</v>
       </c>
       <c r="N17" s="9">
         <v>1.35416666666667E-2</v>
@@ -1816,7 +1822,7 @@
       </c>
       <c r="M18" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45386</v>
+        <v>45387</v>
       </c>
       <c r="N18" s="9">
         <v>1.4583333333333301E-2</v>
@@ -1862,7 +1868,7 @@
       </c>
       <c r="M19" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45387</v>
+        <v>45388</v>
       </c>
       <c r="N19" s="9">
         <v>1.5625E-2</v>
@@ -1908,7 +1914,7 @@
       </c>
       <c r="M20" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45388</v>
+        <v>45389</v>
       </c>
       <c r="N20" s="9">
         <v>1.6666666666666701E-2</v>
@@ -1954,7 +1960,7 @@
       </c>
       <c r="M21" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45389</v>
+        <v>45390</v>
       </c>
       <c r="N21" s="9">
         <v>1.7708333333333302E-2</v>
@@ -2000,7 +2006,7 @@
       </c>
       <c r="M22" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45390</v>
+        <v>45391</v>
       </c>
       <c r="N22" s="9">
         <v>1.8749999999999999E-2</v>
@@ -2046,7 +2052,7 @@
       </c>
       <c r="M23" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45391</v>
+        <v>45392</v>
       </c>
       <c r="N23" s="9">
         <v>1.97916666666667E-2</v>
@@ -2092,7 +2098,7 @@
       </c>
       <c r="M24" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45392</v>
+        <v>45393</v>
       </c>
       <c r="N24" s="9">
         <v>2.0833333333333301E-2</v>
@@ -2138,7 +2144,7 @@
       </c>
       <c r="M25" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45393</v>
+        <v>45394</v>
       </c>
       <c r="N25" s="9">
         <v>2.1874999999999999E-2</v>
@@ -2184,7 +2190,7 @@
       </c>
       <c r="M26" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45394</v>
+        <v>45395</v>
       </c>
       <c r="N26" s="9">
         <v>2.29166666666667E-2</v>
@@ -2230,7 +2236,7 @@
       </c>
       <c r="M27" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45395</v>
+        <v>45396</v>
       </c>
       <c r="N27" s="9">
         <v>2.39583333333333E-2</v>
@@ -2276,7 +2282,7 @@
       </c>
       <c r="M28" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45396</v>
+        <v>45397</v>
       </c>
       <c r="N28" s="9">
         <v>2.5000000000000001E-2</v>
@@ -2322,7 +2328,7 @@
       </c>
       <c r="M29" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45397</v>
+        <v>45398</v>
       </c>
       <c r="N29" s="9">
         <v>2.6041666666666699E-2</v>
@@ -2368,7 +2374,7 @@
       </c>
       <c r="M30" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45398</v>
+        <v>45399</v>
       </c>
       <c r="N30" s="9">
         <v>2.70833333333333E-2</v>
@@ -2414,7 +2420,7 @@
       </c>
       <c r="M31" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45399</v>
+        <v>45400</v>
       </c>
       <c r="N31" s="9">
         <v>2.8125000000000001E-2</v>
@@ -2460,7 +2466,7 @@
       </c>
       <c r="M32" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45400</v>
+        <v>45401</v>
       </c>
       <c r="N32" s="9">
         <v>2.9166666666666698E-2</v>
@@ -2506,7 +2512,7 @@
       </c>
       <c r="M33" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45401</v>
+        <v>45402</v>
       </c>
       <c r="N33" s="9">
         <v>3.0208333333333299E-2</v>
@@ -2552,7 +2558,7 @@
       </c>
       <c r="M34" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45402</v>
+        <v>45403</v>
       </c>
       <c r="N34" s="9">
         <v>3.125E-2</v>
@@ -2598,7 +2604,7 @@
       </c>
       <c r="M35" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45403</v>
+        <v>45404</v>
       </c>
       <c r="N35" s="9">
         <v>3.2291666666666698E-2</v>
@@ -2644,7 +2650,7 @@
       </c>
       <c r="M36" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45404</v>
+        <v>45405</v>
       </c>
       <c r="N36" s="9">
         <v>3.3333333333333298E-2</v>
@@ -2690,7 +2696,7 @@
       </c>
       <c r="M37" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="N37" s="9">
         <v>3.4375000000000003E-2</v>
@@ -2736,7 +2742,7 @@
       </c>
       <c r="M38" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="N38" s="9">
         <v>3.54166666666667E-2</v>
@@ -2782,7 +2788,7 @@
       </c>
       <c r="M39" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45407</v>
+        <v>45408</v>
       </c>
       <c r="N39" s="9">
         <v>3.6458333333333301E-2</v>
@@ -2828,7 +2834,7 @@
       </c>
       <c r="M40" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45408</v>
+        <v>45409</v>
       </c>
       <c r="N40" s="9">
         <v>3.7499999999999999E-2</v>
@@ -2868,7 +2874,7 @@
       <c r="L41" s="11"/>
       <c r="M41" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45409</v>
+        <v>45410</v>
       </c>
       <c r="N41" s="9">
         <v>3.8541666666666703E-2</v>
@@ -2908,7 +2914,7 @@
       <c r="L42" s="11"/>
       <c r="M42" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45410</v>
+        <v>45411</v>
       </c>
       <c r="N42" s="9">
         <v>3.9583333333333297E-2</v>
@@ -2948,7 +2954,7 @@
       <c r="L43" s="11"/>
       <c r="M43" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="N43" s="9">
         <v>4.1666666666666664E-2</v>
@@ -2988,7 +2994,7 @@
       <c r="L44" s="11"/>
       <c r="M44" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45412</v>
+        <v>45413</v>
       </c>
       <c r="N44" s="9">
         <v>4.5833333333333302E-2</v>
@@ -3028,7 +3034,7 @@
       <c r="L45" s="11"/>
       <c r="M45" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45413</v>
+        <v>45414</v>
       </c>
       <c r="N45" s="9">
         <v>4.9999999999999899E-2</v>
@@ -3068,7 +3074,7 @@
       <c r="L46" s="11"/>
       <c r="M46" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="N46" s="9">
         <v>5.4166666666666599E-2</v>
@@ -3108,7 +3114,7 @@
       <c r="L47" s="11"/>
       <c r="M47" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45415</v>
+        <v>45416</v>
       </c>
       <c r="N47" s="9">
         <v>5.83333333333333E-2</v>
@@ -3148,7 +3154,7 @@
       <c r="L48" s="11"/>
       <c r="M48" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45416</v>
+        <v>45417</v>
       </c>
       <c r="N48" s="9">
         <v>6.2499999999999903E-2</v>
@@ -3188,7 +3194,7 @@
       <c r="L49" s="11"/>
       <c r="M49" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45417</v>
+        <v>45418</v>
       </c>
       <c r="N49" s="9">
         <v>6.6666666666666499E-2</v>
@@ -3228,7 +3234,7 @@
       <c r="L50" s="11"/>
       <c r="M50" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="N50" s="9">
         <v>7.0833333333333207E-2</v>
@@ -3268,7 +3274,7 @@
       <c r="L51" s="11"/>
       <c r="M51" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45419</v>
+        <v>45420</v>
       </c>
       <c r="N51" s="9">
         <v>7.4999999999999803E-2</v>
@@ -3308,7 +3314,7 @@
       <c r="L52" s="11"/>
       <c r="M52" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45420</v>
+        <v>45421</v>
       </c>
       <c r="N52" s="9">
         <v>7.9166666666666399E-2</v>
@@ -3348,7 +3354,7 @@
       <c r="L53" s="11"/>
       <c r="M53" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45421</v>
+        <v>45422</v>
       </c>
       <c r="N53" s="9">
         <v>8.3333333333333107E-2</v>
@@ -3388,7 +3394,7 @@
       <c r="L54" s="11"/>
       <c r="M54" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45422</v>
+        <v>45423</v>
       </c>
       <c r="N54" s="9">
         <v>9.0277777777777776E-2</v>
@@ -3428,7 +3434,7 @@
       <c r="L55" s="11"/>
       <c r="M55" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45423</v>
+        <v>45424</v>
       </c>
       <c r="N55" s="9">
         <v>9.7222222222222404E-2</v>
@@ -3468,7 +3474,7 @@
       <c r="L56" s="11"/>
       <c r="M56" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45424</v>
+        <v>45425</v>
       </c>
       <c r="N56" s="9">
         <v>0.104166666666667</v>
@@ -3508,7 +3514,7 @@
       <c r="L57" s="11"/>
       <c r="M57" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45425</v>
+        <v>45426</v>
       </c>
       <c r="N57" s="9">
         <v>0.11111111111111199</v>
@@ -3548,7 +3554,7 @@
       <c r="L58" s="11"/>
       <c r="M58" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45426</v>
+        <v>45427</v>
       </c>
       <c r="N58" s="9">
         <v>0.118055555555556</v>
@@ -3588,7 +3594,7 @@
       <c r="L59" s="11"/>
       <c r="M59" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45427</v>
+        <v>45428</v>
       </c>
       <c r="N59" s="9">
         <v>0.125000000000001</v>
@@ -3628,7 +3634,7 @@
       <c r="L60" s="11"/>
       <c r="M60" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45428</v>
+        <v>45429</v>
       </c>
       <c r="N60" s="9">
         <v>0.131944444444446</v>
@@ -3668,7 +3674,7 @@
       <c r="L61" s="11"/>
       <c r="M61" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45429</v>
+        <v>45430</v>
       </c>
       <c r="N61" s="9">
         <v>0.138888888888891</v>

</xml_diff>

<commit_message>
updating layout and track
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FED5C3-0282-43D3-AF54-590E22370A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3BBA84-42BF-47AD-BB47-A58939F8CA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -910,7 +910,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1389,7 +1389,9 @@
       <c r="C10" s="9">
         <v>7.2916666666666703E-3</v>
       </c>
-      <c r="D10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>4</v>
+      </c>
       <c r="E10" s="11">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Build New Issue Page
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8EFC2B-C6AF-4490-B354-ED119CD22910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D977E72-EC48-4E81-B63E-CD99CA07DBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -874,7 +874,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -1771,7 +1771,9 @@
       <c r="C18" s="1">
         <v>1.5625E-2</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="E18" s="2">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Customize Radiux UI Theme
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D977E72-EC48-4E81-B63E-CD99CA07DBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7440CBCE-681D-46D5-A872-89873CD1139C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -874,7 +874,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -940,11 +940,11 @@
       <c r="D2" s="16"/>
       <c r="E2" s="6">
         <f>(E3+(F3/60))/60</f>
-        <v>0.84555555555555562</v>
+        <v>0.92666666666666664</v>
       </c>
       <c r="F2" s="7">
         <f>(E3+(F3/60))</f>
-        <v>50.733333333333334</v>
+        <v>55.6</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
@@ -986,11 +986,11 @@
       </c>
       <c r="E3" s="8">
         <f>SUM(E4:E71)</f>
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F3" s="8">
         <f>SUM(F4:F71)</f>
-        <v>584</v>
+        <v>636</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>0</v>
@@ -1823,9 +1823,15 @@
       <c r="C19" s="1">
         <v>1.6666666666666701E-2</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="D19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="2">
+        <v>4</v>
+      </c>
+      <c r="F19" s="2">
+        <v>52</v>
+      </c>
       <c r="G19" s="15">
         <v>45346</v>
       </c>

</xml_diff>

<commit_message>
Add A mark down editor
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f7c3dc73fd6fbfd/Desktop/dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7440CBCE-681D-46D5-A872-89873CD1139C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{7440CBCE-681D-46D5-A872-89873CD1139C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4C2FEF2-E1AE-43B3-BF2F-12BC74F277A1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Mastering Next.js 13 with TypeScript</t>
-  </si>
-  <si>
     <t>Next.js 14 Admin Dashboard Tutorial Fullstack Next.js 14 Project with Server Actions</t>
   </si>
   <si>
@@ -63,7 +60,10 @@
     <t>MIN</t>
   </si>
   <si>
-    <t>Build a Full-Stack App with Next.js, Tailwind, Radix UI, and Prisma</t>
+    <t>Mastering Next.js 13 with TypeScript - PART 1</t>
+  </si>
+  <si>
+    <t>Build a Full-Stack App with Next.js, Tailwind, Radix UI, and Prisma - PART 2</t>
   </si>
 </sst>
 </file>
@@ -569,8 +569,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A42150A-74BB-4659-8BE3-C38AE4DF6F2F}" name="Table22" displayName="Table22" ref="G3:J71" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="G3:J71" xr:uid="{9A42150A-74BB-4659-8BE3-C38AE4DF6F2F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A42150A-74BB-4659-8BE3-C38AE4DF6F2F}" name="Table22" displayName="Table22" ref="A3:D71" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A3:D71" xr:uid="{9A42150A-74BB-4659-8BE3-C38AE4DF6F2F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E47A06B2-66D0-4A3B-94F5-F413F13FA3D5}" name="Date" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{263AAFE7-CED9-4BC8-BDF4-682077A1A32F}" name="FROM" dataDxfId="14"/>
@@ -595,8 +595,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E2833A92-15F0-45DF-8153-A7603B424774}" name="Table225" displayName="Table225" ref="A3:D71" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A3:D71" xr:uid="{E2833A92-15F0-45DF-8153-A7603B424774}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E2833A92-15F0-45DF-8153-A7603B424774}" name="Table225" displayName="Table225" ref="G3:J71" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="G3:J71" xr:uid="{E2833A92-15F0-45DF-8153-A7603B424774}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F939511D-5FD6-4F93-B2DB-3FBFE1C3FCD5}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{1AE9D2F2-DAC2-4413-9B1B-4723A3CDD042}" name="FROM" dataDxfId="2"/>
@@ -873,22 +873,22 @@
   <dimension ref="A1:R72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5546875" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.77734375" style="13" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" style="11" customWidth="1"/>
     <col min="5" max="5" width="12.77734375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="41.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.77734375" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.77734375" style="13" customWidth="1"/>
     <col min="10" max="10" width="12.77734375" style="11" customWidth="1"/>
     <col min="11" max="11" width="12.77734375" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" style="14" customWidth="1"/>
     <col min="13" max="13" width="36.77734375" style="11" bestFit="1" customWidth="1"/>
     <col min="14" max="17" width="12.77734375" style="11" customWidth="1"/>
     <col min="18" max="18" width="8.77734375" style="11" customWidth="1"/>
@@ -896,67 +896,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>6</v>
       </c>
       <c r="N1" s="16"/>
       <c r="O1" s="16"/>
       <c r="P1" s="16"/>
       <c r="Q1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:18" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="6">
         <f>(E3+(F3/60))/60</f>
-        <v>0.92666666666666664</v>
+        <v>2.3347222222222226</v>
       </c>
       <c r="F2" s="7">
         <f>(E3+(F3/60))</f>
-        <v>55.6</v>
-      </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
+        <v>140.08333333333334</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
       <c r="K2" s="6">
         <f>(K3+(L3/60))/60</f>
-        <v>2.3347222222222226</v>
+        <v>1.1205555555555555</v>
       </c>
       <c r="L2" s="7">
         <f>(K3+(L3/60))</f>
-        <v>140.08333333333334</v>
+        <v>67.233333333333334</v>
       </c>
       <c r="M2" s="16"/>
       <c r="N2" s="16"/>
@@ -986,11 +986,11 @@
       </c>
       <c r="E3" s="8">
         <f>SUM(E4:E71)</f>
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="F3" s="8">
         <f>SUM(F4:F71)</f>
-        <v>636</v>
+        <v>965</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>0</v>
@@ -1006,11 +1006,11 @@
       </c>
       <c r="K3" s="8">
         <f>SUM(K4:K71)</f>
-        <v>124</v>
+        <v>55</v>
       </c>
       <c r="L3" s="8">
         <f>SUM(L4:L71)</f>
-        <v>965</v>
+        <v>734</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>0</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="4" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
-        <v>45374</v>
+        <v>45331</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -1043,36 +1043,36 @@
       <c r="C4" s="1">
         <v>1.0416666666666667E-3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="G4" s="15">
-        <v>45331</v>
+        <v>45374</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>1.0416666666666667E-3</v>
-      </c>
-      <c r="J4" s="10" t="s">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="K4" s="2">
         <v>2</v>
       </c>
       <c r="L4" s="2">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="M4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45379</v>
+        <v>45380</v>
       </c>
       <c r="N4" s="1">
         <v>0</v>
@@ -1086,8 +1086,7 @@
     </row>
     <row r="5" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
-        <f>A4+1</f>
-        <v>45375</v>
+        <v>45332</v>
       </c>
       <c r="B5" s="1">
         <v>1.0416666666666667E-3</v>
@@ -1095,36 +1094,37 @@
       <c r="C5" s="1">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="15">
+        <f>G4+1</f>
+        <v>45375</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>4.1666666666666701E-3</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
+      <c r="L5" s="2">
         <v>48</v>
-      </c>
-      <c r="G5" s="15">
-        <v>45332</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1.0416666666666667E-3</v>
-      </c>
-      <c r="I5" s="1">
-        <v>2.0833333333333333E-3</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
-        <v>4</v>
       </c>
       <c r="M5" s="15">
         <f ca="1">M4+1</f>
-        <v>45380</v>
+        <v>45381</v>
       </c>
       <c r="N5" s="1">
         <v>1.0416666666666667E-3</v>
@@ -1138,8 +1138,7 @@
     </row>
     <row r="6" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
-        <f t="shared" ref="A6:A69" si="0">A5+1</f>
-        <v>45376</v>
+        <v>45333</v>
       </c>
       <c r="B6" s="1">
         <v>2.0833333333333298E-3</v>
@@ -1147,36 +1146,37 @@
       <c r="C6" s="1">
         <v>3.1250000000000002E-3</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>25</v>
+      </c>
+      <c r="G6" s="15">
+        <f t="shared" ref="G6:G69" si="0">G5+1</f>
+        <v>45376</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4.1666666666666701E-3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="2">
+      <c r="L6" s="2">
         <v>38</v>
-      </c>
-      <c r="G6" s="15">
-        <v>45333</v>
-      </c>
-      <c r="H6" s="1">
-        <v>2.0833333333333298E-3</v>
-      </c>
-      <c r="I6" s="1">
-        <v>3.1250000000000002E-3</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1</v>
-      </c>
-      <c r="L6" s="2">
-        <v>25</v>
       </c>
       <c r="M6" s="15">
         <f t="shared" ref="M6:M61" ca="1" si="1">M5+1</f>
-        <v>45381</v>
+        <v>45382</v>
       </c>
       <c r="N6" s="1">
         <v>2.0833333333333298E-3</v>
@@ -1190,8 +1190,7 @@
     </row>
     <row r="7" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
-        <f t="shared" si="0"/>
-        <v>45377</v>
+        <v>45334</v>
       </c>
       <c r="B7" s="1">
         <v>3.1250000000000002E-3</v>
@@ -1199,36 +1198,37 @@
       <c r="C7" s="1">
         <v>4.1666666666666701E-3</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="G7" s="15">
-        <v>45334</v>
+        <f t="shared" si="0"/>
+        <v>45377</v>
       </c>
       <c r="H7" s="1">
-        <v>3.1250000000000002E-3</v>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="I7" s="1">
-        <v>4.1666666666666701E-3</v>
-      </c>
-      <c r="J7" s="10" t="s">
+        <v>8.3333333333333402E-3</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>4</v>
       </c>
       <c r="K7" s="3">
         <v>0</v>
       </c>
       <c r="L7" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="M7" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45382</v>
+        <v>45383</v>
       </c>
       <c r="N7" s="1">
         <v>3.1250000000000002E-3</v>
@@ -1242,8 +1242,7 @@
     </row>
     <row r="8" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
-        <f t="shared" si="0"/>
-        <v>45378</v>
+        <v>45335</v>
       </c>
       <c r="B8" s="1">
         <v>4.1666666666666701E-3</v>
@@ -1251,36 +1250,37 @@
       <c r="C8" s="1">
         <v>5.20833333333334E-3</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
       </c>
       <c r="F8" s="2">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G8" s="15">
-        <v>45335</v>
+        <f t="shared" si="0"/>
+        <v>45378</v>
       </c>
       <c r="H8" s="1">
-        <v>4.1666666666666701E-3</v>
+        <v>8.3333333333333297E-3</v>
       </c>
       <c r="I8" s="1">
-        <v>5.20833333333334E-3</v>
-      </c>
-      <c r="J8" s="10" t="s">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>4</v>
       </c>
       <c r="K8" s="2">
         <v>2</v>
       </c>
       <c r="L8" s="2">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="M8" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45383</v>
+        <v>45384</v>
       </c>
       <c r="N8" s="1">
         <v>4.1666666666666701E-3</v>
@@ -1294,8 +1294,7 @@
     </row>
     <row r="9" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
-        <f t="shared" si="0"/>
-        <v>45379</v>
+        <v>45336</v>
       </c>
       <c r="B9" s="1">
         <v>5.2083333333333296E-3</v>
@@ -1303,36 +1302,37 @@
       <c r="C9" s="1">
         <v>6.2500000000000003E-3</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" s="2">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G9" s="15">
-        <v>45336</v>
+        <f t="shared" si="0"/>
+        <v>45379</v>
       </c>
       <c r="H9" s="1">
-        <v>5.2083333333333296E-3</v>
+        <v>1.0416666666666701E-2</v>
       </c>
       <c r="I9" s="1">
-        <v>6.2500000000000003E-3</v>
-      </c>
-      <c r="J9" s="10" t="s">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="J9" s="9" t="s">
         <v>4</v>
       </c>
       <c r="K9" s="2">
         <v>1</v>
       </c>
       <c r="L9" s="2">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="M9" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45384</v>
+        <v>45385</v>
       </c>
       <c r="N9" s="1">
         <v>5.2083333333333296E-3</v>
@@ -1346,8 +1346,7 @@
     </row>
     <row r="10" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
-        <f t="shared" si="0"/>
-        <v>45380</v>
+        <v>45337</v>
       </c>
       <c r="B10" s="1">
         <v>6.2500000000000003E-3</v>
@@ -1355,36 +1354,37 @@
       <c r="C10" s="1">
         <v>7.2916666666666703E-3</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
       </c>
       <c r="F10" s="2">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="G10" s="15">
-        <v>45337</v>
+        <f t="shared" si="0"/>
+        <v>45380</v>
       </c>
       <c r="H10" s="1">
-        <v>6.2500000000000003E-3</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="I10" s="1">
-        <v>7.2916666666666703E-3</v>
-      </c>
-      <c r="J10" s="10" t="s">
+        <v>1.4583333333333301E-2</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>4</v>
       </c>
       <c r="K10" s="2">
         <v>2</v>
       </c>
       <c r="L10" s="2">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="M10" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45385</v>
+        <v>45386</v>
       </c>
       <c r="N10" s="1">
         <v>6.2500000000000003E-3</v>
@@ -1398,8 +1398,7 @@
     </row>
     <row r="11" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
-        <f t="shared" si="0"/>
-        <v>45381</v>
+        <v>45338</v>
       </c>
       <c r="B11" s="1">
         <v>7.2916666666666703E-3</v>
@@ -1407,36 +1406,37 @@
       <c r="C11" s="1">
         <v>8.3333333333333402E-3</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>49</v>
+      </c>
+      <c r="G11" s="15">
+        <f t="shared" si="0"/>
+        <v>45381</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.4583333333333301E-2</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1.6666666666666701E-2</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="2">
         <v>8</v>
       </c>
-      <c r="F11" s="2">
+      <c r="L11" s="2">
         <v>52</v>
       </c>
-      <c r="G11" s="15">
-        <v>45338</v>
-      </c>
-      <c r="H11" s="1">
-        <v>7.2916666666666703E-3</v>
-      </c>
-      <c r="I11" s="1">
-        <v>8.3333333333333402E-3</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="2">
-        <v>2</v>
-      </c>
-      <c r="L11" s="2">
-        <v>49</v>
-      </c>
       <c r="M11" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45386</v>
+        <v>45387</v>
       </c>
       <c r="N11" s="1">
         <v>7.2916666666666703E-3</v>
@@ -1450,8 +1450,7 @@
     </row>
     <row r="12" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
-        <f t="shared" si="0"/>
-        <v>45382</v>
+        <v>45339</v>
       </c>
       <c r="B12" s="1">
         <v>8.3333333333333297E-3</v>
@@ -1459,36 +1458,37 @@
       <c r="C12" s="1">
         <v>9.3749999999999997E-3</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>15</v>
+      </c>
+      <c r="G12" s="15">
+        <f t="shared" si="0"/>
+        <v>45382</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.6666666666666701E-2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="2">
         <v>6</v>
       </c>
-      <c r="F12" s="2">
+      <c r="L12" s="2">
         <v>17</v>
       </c>
-      <c r="G12" s="15">
-        <v>45339</v>
-      </c>
-      <c r="H12" s="1">
-        <v>8.3333333333333297E-3</v>
-      </c>
-      <c r="I12" s="1">
-        <v>9.3749999999999997E-3</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K12" s="2">
-        <v>5</v>
-      </c>
-      <c r="L12" s="2">
-        <v>15</v>
-      </c>
       <c r="M12" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45387</v>
+        <v>45388</v>
       </c>
       <c r="N12" s="1">
         <v>8.3333333333333297E-3</v>
@@ -1502,8 +1502,7 @@
     </row>
     <row r="13" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
-        <f t="shared" si="0"/>
-        <v>45383</v>
+        <v>45340</v>
       </c>
       <c r="B13" s="1">
         <v>9.3749999999999997E-3</v>
@@ -1511,36 +1510,37 @@
       <c r="C13" s="1">
         <v>1.0416666666666701E-2</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="2">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2">
+        <v>13</v>
+      </c>
+      <c r="G13" s="15">
+        <f t="shared" si="0"/>
+        <v>45383</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="2">
         <v>1</v>
       </c>
-      <c r="F13" s="2">
+      <c r="L13" s="2">
         <v>58</v>
       </c>
-      <c r="G13" s="15">
-        <v>45340</v>
-      </c>
-      <c r="H13" s="1">
-        <v>9.3749999999999997E-3</v>
-      </c>
-      <c r="I13" s="1">
-        <v>1.0416666666666701E-2</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13" s="2">
-        <v>8</v>
-      </c>
-      <c r="L13" s="2">
-        <v>13</v>
-      </c>
       <c r="M13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45388</v>
+        <v>45389</v>
       </c>
       <c r="N13" s="1">
         <v>9.3749999999999997E-3</v>
@@ -1554,8 +1554,7 @@
     </row>
     <row r="14" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
-        <f t="shared" si="0"/>
-        <v>45384</v>
+        <v>45341</v>
       </c>
       <c r="B14" s="1">
         <v>1.0416666666666701E-2</v>
@@ -1563,36 +1562,37 @@
       <c r="C14" s="1">
         <v>1.14583333333334E-2</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="2">
+        <v>6</v>
+      </c>
+      <c r="F14" s="2">
+        <v>4</v>
+      </c>
+      <c r="G14" s="15">
+        <f t="shared" si="0"/>
+        <v>45384</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2.29166666666667E-2</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="2">
+      <c r="L14" s="2">
         <v>45</v>
       </c>
-      <c r="G14" s="15">
-        <v>45341</v>
-      </c>
-      <c r="H14" s="1">
-        <v>1.0416666666666701E-2</v>
-      </c>
-      <c r="I14" s="1">
-        <v>1.14583333333334E-2</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="2">
-        <v>6</v>
-      </c>
-      <c r="L14" s="2">
-        <v>4</v>
-      </c>
       <c r="M14" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45389</v>
+        <v>45390</v>
       </c>
       <c r="N14" s="1">
         <v>1.0416666666666701E-2</v>
@@ -1606,8 +1606,7 @@
     </row>
     <row r="15" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
-        <f t="shared" si="0"/>
-        <v>45385</v>
+        <v>45342</v>
       </c>
       <c r="B15" s="1">
         <v>1.14583333333333E-2</v>
@@ -1615,36 +1614,37 @@
       <c r="C15" s="1">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="2">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>25</v>
+      </c>
+      <c r="G15" s="15">
+        <f t="shared" si="0"/>
+        <v>45385</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2.29166666666667E-2</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="2">
         <v>6</v>
       </c>
-      <c r="F15" s="2">
+      <c r="L15" s="2">
         <v>40</v>
       </c>
-      <c r="G15" s="15">
-        <v>45342</v>
-      </c>
-      <c r="H15" s="1">
-        <v>1.14583333333333E-2</v>
-      </c>
-      <c r="I15" s="1">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K15" s="2">
-        <v>2</v>
-      </c>
-      <c r="L15" s="2">
-        <v>25</v>
-      </c>
       <c r="M15" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45390</v>
+        <v>45391</v>
       </c>
       <c r="N15" s="1">
         <v>1.14583333333333E-2</v>
@@ -1658,8 +1658,7 @@
     </row>
     <row r="16" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
-        <f t="shared" si="0"/>
-        <v>45386</v>
+        <v>45343</v>
       </c>
       <c r="B16" s="1">
         <v>1.2500000000000001E-2</v>
@@ -1667,36 +1666,37 @@
       <c r="C16" s="1">
         <v>1.35416666666667E-2</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="2">
+        <v>4</v>
+      </c>
+      <c r="F16" s="2">
+        <v>9</v>
+      </c>
+      <c r="G16" s="15">
+        <f t="shared" si="0"/>
+        <v>45386</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2.70833333333333E-2</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="2">
         <v>6</v>
       </c>
-      <c r="F16" s="2">
+      <c r="L16" s="2">
         <v>54</v>
       </c>
-      <c r="G16" s="15">
-        <v>45343</v>
-      </c>
-      <c r="H16" s="1">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="I16" s="1">
-        <v>1.35416666666667E-2</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" s="2">
-        <v>4</v>
-      </c>
-      <c r="L16" s="2">
-        <v>9</v>
-      </c>
       <c r="M16" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45391</v>
+        <v>45392</v>
       </c>
       <c r="N16" s="1">
         <v>1.2500000000000001E-2</v>
@@ -1710,8 +1710,7 @@
     </row>
     <row r="17" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
-        <f t="shared" si="0"/>
-        <v>45387</v>
+        <v>45344</v>
       </c>
       <c r="B17" s="1">
         <v>1.35416666666667E-2</v>
@@ -1719,36 +1718,37 @@
       <c r="C17" s="1">
         <v>1.4583333333333399E-2</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>20</v>
+      </c>
+      <c r="G17" s="15">
+        <f t="shared" si="0"/>
+        <v>45387</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2.70833333333333E-2</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2.9166666666666698E-2</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="2">
         <v>2</v>
       </c>
-      <c r="F17" s="2">
+      <c r="L17" s="2">
         <v>32</v>
       </c>
-      <c r="G17" s="15">
-        <v>45344</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1.35416666666667E-2</v>
-      </c>
-      <c r="I17" s="1">
-        <v>1.4583333333333399E-2</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2">
-        <v>20</v>
-      </c>
       <c r="M17" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45392</v>
+        <v>45393</v>
       </c>
       <c r="N17" s="1">
         <v>1.35416666666667E-2</v>
@@ -1762,8 +1762,7 @@
     </row>
     <row r="18" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
-        <f t="shared" si="0"/>
-        <v>45388</v>
+        <v>45345</v>
       </c>
       <c r="B18" s="1">
         <v>1.4583333333333301E-2</v>
@@ -1771,36 +1770,37 @@
       <c r="C18" s="1">
         <v>1.5625E-2</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F18" s="2">
+        <v>34</v>
+      </c>
+      <c r="G18" s="15">
+        <f t="shared" si="0"/>
+        <v>45388</v>
+      </c>
+      <c r="H18" s="1">
+        <v>2.9166666666666698E-2</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="2">
+        <v>4</v>
+      </c>
+      <c r="L18" s="2">
         <v>57</v>
       </c>
-      <c r="G18" s="15">
-        <v>45345</v>
-      </c>
-      <c r="H18" s="1">
-        <v>1.4583333333333301E-2</v>
-      </c>
-      <c r="I18" s="1">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K18" s="2">
-        <v>2</v>
-      </c>
-      <c r="L18" s="2">
-        <v>34</v>
-      </c>
       <c r="M18" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45393</v>
+        <v>45394</v>
       </c>
       <c r="N18" s="1">
         <v>1.4583333333333301E-2</v>
@@ -1814,8 +1814,7 @@
     </row>
     <row r="19" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
-        <f t="shared" si="0"/>
-        <v>45389</v>
+        <v>45346</v>
       </c>
       <c r="B19" s="1">
         <v>1.5625E-2</v>
@@ -1823,36 +1822,37 @@
       <c r="C19" s="1">
         <v>1.6666666666666701E-2</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="2">
         <v>4</v>
       </c>
       <c r="F19" s="2">
+        <v>27</v>
+      </c>
+      <c r="G19" s="15">
+        <f t="shared" si="0"/>
+        <v>45389</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="2">
+        <v>4</v>
+      </c>
+      <c r="L19" s="2">
         <v>52</v>
       </c>
-      <c r="G19" s="15">
-        <v>45346</v>
-      </c>
-      <c r="H19" s="1">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="I19" s="1">
-        <v>1.6666666666666701E-2</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K19" s="2">
-        <v>4</v>
-      </c>
-      <c r="L19" s="2">
-        <v>27</v>
-      </c>
       <c r="M19" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45394</v>
+        <v>45395</v>
       </c>
       <c r="N19" s="1">
         <v>1.5625E-2</v>
@@ -1866,8 +1866,7 @@
     </row>
     <row r="20" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
-        <f t="shared" si="0"/>
-        <v>45390</v>
+        <v>45347</v>
       </c>
       <c r="B20" s="1">
         <v>1.6666666666666701E-2</v>
@@ -1875,30 +1874,37 @@
       <c r="C20" s="1">
         <v>1.7708333333333399E-2</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="D20" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="2">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2">
+        <v>39</v>
+      </c>
       <c r="G20" s="15">
-        <v>45347</v>
+        <f t="shared" si="0"/>
+        <v>45390</v>
       </c>
       <c r="H20" s="1">
-        <v>1.6666666666666701E-2</v>
+        <v>3.3333333333333298E-2</v>
       </c>
       <c r="I20" s="1">
-        <v>1.7708333333333399E-2</v>
-      </c>
-      <c r="J20" s="10" t="s">
+        <v>3.54166666666667E-2</v>
+      </c>
+      <c r="J20" s="9" t="s">
         <v>4</v>
       </c>
       <c r="K20" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L20" s="2">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="M20" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45395</v>
+        <v>45396</v>
       </c>
       <c r="N20" s="1">
         <v>1.6666666666666701E-2</v>
@@ -1912,8 +1918,7 @@
     </row>
     <row r="21" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
-        <f t="shared" si="0"/>
-        <v>45391</v>
+        <v>45348</v>
       </c>
       <c r="B21" s="1">
         <v>1.7708333333333302E-2</v>
@@ -1921,30 +1926,37 @@
       <c r="C21" s="1">
         <v>1.8749999999999999E-2</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="D21" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2">
+        <v>7</v>
+      </c>
+      <c r="F21" s="2">
+        <v>17</v>
+      </c>
       <c r="G21" s="15">
-        <v>45348</v>
+        <f t="shared" si="0"/>
+        <v>45391</v>
       </c>
       <c r="H21" s="1">
-        <v>1.7708333333333302E-2</v>
+        <v>3.54166666666667E-2</v>
       </c>
       <c r="I21" s="1">
-        <v>1.8749999999999999E-2</v>
-      </c>
-      <c r="J21" s="10" t="s">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="J21" s="9" t="s">
         <v>4</v>
       </c>
       <c r="K21" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L21" s="2">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="M21" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45396</v>
+        <v>45397</v>
       </c>
       <c r="N21" s="1">
         <v>1.7708333333333302E-2</v>
@@ -1958,8 +1970,7 @@
     </row>
     <row r="22" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
-        <f t="shared" si="0"/>
-        <v>45392</v>
+        <v>45349</v>
       </c>
       <c r="B22" s="1">
         <v>1.8749999999999999E-2</v>
@@ -1967,30 +1978,35 @@
       <c r="C22" s="1">
         <v>1.97916666666667E-2</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="D22" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>27</v>
+      </c>
       <c r="G22" s="15">
-        <v>45349</v>
+        <f t="shared" si="0"/>
+        <v>45392</v>
       </c>
       <c r="H22" s="1">
-        <v>1.8749999999999999E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="I22" s="1">
-        <v>1.97916666666667E-2</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>4</v>
-      </c>
+        <v>3.9583333333333401E-2</v>
+      </c>
+      <c r="J22" s="10"/>
       <c r="K22" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L22" s="2">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="M22" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45397</v>
+        <v>45398</v>
       </c>
       <c r="N22" s="1">
         <v>1.8749999999999999E-2</v>
@@ -2004,8 +2020,7 @@
     </row>
     <row r="23" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
-        <f t="shared" si="0"/>
-        <v>45393</v>
+        <v>45350</v>
       </c>
       <c r="B23" s="1">
         <v>1.97916666666667E-2</v>
@@ -2013,30 +2028,31 @@
       <c r="C23" s="1">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="D23" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3</v>
+      </c>
+      <c r="F23" s="2">
+        <v>54</v>
+      </c>
       <c r="G23" s="15">
-        <v>45350</v>
+        <f t="shared" si="0"/>
+        <v>45393</v>
       </c>
       <c r="H23" s="1">
-        <v>1.97916666666667E-2</v>
+        <v>3.9583333333333297E-2</v>
       </c>
       <c r="I23" s="1">
-        <v>2.0833333333333402E-2</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K23" s="2">
-        <v>3</v>
-      </c>
-      <c r="L23" s="2">
-        <v>54</v>
-      </c>
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
       <c r="M23" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45398</v>
+        <v>45399</v>
       </c>
       <c r="N23" s="1">
         <v>1.97916666666667E-2</v>
@@ -2050,8 +2066,7 @@
     </row>
     <row r="24" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
-        <f t="shared" si="0"/>
-        <v>45394</v>
+        <v>45351</v>
       </c>
       <c r="B24" s="1">
         <v>2.0833333333333301E-2</v>
@@ -2059,30 +2074,31 @@
       <c r="C24" s="1">
         <v>2.1874999999999999E-2</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="D24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="2">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2">
+        <v>59</v>
+      </c>
       <c r="G24" s="15">
-        <v>45351</v>
+        <f t="shared" si="0"/>
+        <v>45394</v>
       </c>
       <c r="H24" s="1">
-        <v>2.0833333333333301E-2</v>
+        <v>4.1666666666666699E-2</v>
       </c>
       <c r="I24" s="1">
-        <v>2.1874999999999999E-2</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K24" s="2">
-        <v>3</v>
-      </c>
-      <c r="L24" s="2">
-        <v>59</v>
-      </c>
+        <v>4.3749999999999997E-2</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
       <c r="M24" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45399</v>
+        <v>45400</v>
       </c>
       <c r="N24" s="1">
         <v>2.0833333333333301E-2</v>
@@ -2096,8 +2112,7 @@
     </row>
     <row r="25" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
-        <f t="shared" si="0"/>
-        <v>45395</v>
+        <v>45352</v>
       </c>
       <c r="B25" s="1">
         <v>2.1874999999999999E-2</v>
@@ -2105,30 +2120,31 @@
       <c r="C25" s="1">
         <v>2.29166666666667E-2</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="D25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2">
+        <v>54</v>
+      </c>
       <c r="G25" s="15">
-        <v>45352</v>
+        <f t="shared" si="0"/>
+        <v>45395</v>
       </c>
       <c r="H25" s="1">
-        <v>2.1874999999999999E-2</v>
+        <v>4.3749999999999997E-2</v>
       </c>
       <c r="I25" s="1">
-        <v>2.29166666666667E-2</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K25" s="2">
-        <v>2</v>
-      </c>
-      <c r="L25" s="2">
-        <v>54</v>
-      </c>
+        <v>4.5833333333333399E-2</v>
+      </c>
+      <c r="J25" s="10"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
       <c r="M25" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45400</v>
+        <v>45401</v>
       </c>
       <c r="N25" s="1">
         <v>2.1874999999999999E-2</v>
@@ -2142,8 +2158,7 @@
     </row>
     <row r="26" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
-        <f t="shared" si="0"/>
-        <v>45396</v>
+        <v>45353</v>
       </c>
       <c r="B26" s="1">
         <v>2.29166666666667E-2</v>
@@ -2151,30 +2166,31 @@
       <c r="C26" s="1">
         <v>2.3958333333333401E-2</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="D26" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2">
+        <v>7</v>
+      </c>
+      <c r="F26" s="2">
+        <v>9</v>
+      </c>
       <c r="G26" s="15">
-        <v>45353</v>
+        <f t="shared" si="0"/>
+        <v>45396</v>
       </c>
       <c r="H26" s="1">
-        <v>2.29166666666667E-2</v>
+        <v>4.5833333333333302E-2</v>
       </c>
       <c r="I26" s="1">
-        <v>2.3958333333333401E-2</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K26" s="2">
-        <v>7</v>
-      </c>
-      <c r="L26" s="2">
-        <v>9</v>
-      </c>
+        <v>4.7916666666666698E-2</v>
+      </c>
+      <c r="J26" s="10"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
       <c r="M26" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45401</v>
+        <v>45402</v>
       </c>
       <c r="N26" s="1">
         <v>2.29166666666667E-2</v>
@@ -2188,8 +2204,7 @@
     </row>
     <row r="27" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
-        <f t="shared" si="0"/>
-        <v>45397</v>
+        <v>45354</v>
       </c>
       <c r="B27" s="1">
         <v>2.39583333333333E-2</v>
@@ -2197,30 +2212,31 @@
       <c r="C27" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="D27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="2">
+        <v>8</v>
+      </c>
+      <c r="F27" s="2">
+        <v>11</v>
+      </c>
       <c r="G27" s="15">
-        <v>45354</v>
+        <f t="shared" si="0"/>
+        <v>45397</v>
       </c>
       <c r="H27" s="1">
-        <v>2.39583333333333E-2</v>
+        <v>4.7916666666666698E-2</v>
       </c>
       <c r="I27" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="J27" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="2">
-        <v>8</v>
-      </c>
-      <c r="L27" s="2">
-        <v>11</v>
-      </c>
+        <v>0.05</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
       <c r="M27" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45402</v>
+        <v>45403</v>
       </c>
       <c r="N27" s="1">
         <v>2.39583333333333E-2</v>
@@ -2234,8 +2250,7 @@
     </row>
     <row r="28" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
-        <f t="shared" si="0"/>
-        <v>45398</v>
+        <v>45355</v>
       </c>
       <c r="B28" s="1">
         <v>2.5000000000000001E-2</v>
@@ -2243,30 +2258,31 @@
       <c r="C28" s="1">
         <v>2.6041666666666699E-2</v>
       </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="D28" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="2">
+        <v>3</v>
+      </c>
+      <c r="F28" s="2">
+        <v>28</v>
+      </c>
       <c r="G28" s="15">
-        <v>45355</v>
+        <f t="shared" si="0"/>
+        <v>45398</v>
       </c>
       <c r="H28" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="I28" s="1">
-        <v>2.6041666666666699E-2</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K28" s="2">
-        <v>3</v>
-      </c>
-      <c r="L28" s="2">
-        <v>28</v>
-      </c>
+        <v>5.2083333333333398E-2</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
       <c r="M28" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45403</v>
+        <v>45404</v>
       </c>
       <c r="N28" s="1">
         <v>2.5000000000000001E-2</v>
@@ -2280,8 +2296,7 @@
     </row>
     <row r="29" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
-        <f t="shared" si="0"/>
-        <v>45399</v>
+        <v>45356</v>
       </c>
       <c r="B29" s="1">
         <v>2.6041666666666699E-2</v>
@@ -2289,30 +2304,31 @@
       <c r="C29" s="1">
         <v>2.70833333333334E-2</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="D29" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2">
+        <v>3</v>
+      </c>
+      <c r="F29" s="2">
+        <v>11</v>
+      </c>
       <c r="G29" s="15">
-        <v>45356</v>
+        <f t="shared" si="0"/>
+        <v>45399</v>
       </c>
       <c r="H29" s="1">
-        <v>2.6041666666666699E-2</v>
+        <v>5.2083333333333301E-2</v>
       </c>
       <c r="I29" s="1">
-        <v>2.70833333333334E-2</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="2">
-        <v>3</v>
-      </c>
-      <c r="L29" s="2">
-        <v>11</v>
-      </c>
+        <v>5.4166666666666703E-2</v>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
       <c r="M29" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45404</v>
+        <v>45405</v>
       </c>
       <c r="N29" s="1">
         <v>2.6041666666666699E-2</v>
@@ -2326,8 +2342,7 @@
     </row>
     <row r="30" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
-        <f t="shared" si="0"/>
-        <v>45400</v>
+        <v>45357</v>
       </c>
       <c r="B30" s="1">
         <v>2.70833333333333E-2</v>
@@ -2335,30 +2350,31 @@
       <c r="C30" s="1">
         <v>2.8125000000000001E-2</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="D30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="2">
+        <v>6</v>
+      </c>
+      <c r="F30" s="2">
+        <v>14</v>
+      </c>
       <c r="G30" s="15">
-        <v>45357</v>
+        <f t="shared" si="0"/>
+        <v>45400</v>
       </c>
       <c r="H30" s="1">
-        <v>2.70833333333333E-2</v>
+        <v>5.4166666666666703E-2</v>
       </c>
       <c r="I30" s="1">
-        <v>2.8125000000000001E-2</v>
-      </c>
-      <c r="J30" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30" s="2">
-        <v>6</v>
-      </c>
-      <c r="L30" s="2">
-        <v>14</v>
-      </c>
+        <v>5.6250000000000099E-2</v>
+      </c>
+      <c r="J30" s="10"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
       <c r="M30" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="N30" s="1">
         <v>2.70833333333333E-2</v>
@@ -2372,8 +2388,7 @@
     </row>
     <row r="31" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
-        <f t="shared" si="0"/>
-        <v>45401</v>
+        <v>45358</v>
       </c>
       <c r="B31" s="1">
         <v>2.8125000000000001E-2</v>
@@ -2381,30 +2396,31 @@
       <c r="C31" s="1">
         <v>2.9166666666666698E-2</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="D31" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2">
+        <v>41</v>
+      </c>
       <c r="G31" s="15">
-        <v>45358</v>
+        <f t="shared" si="0"/>
+        <v>45401</v>
       </c>
       <c r="H31" s="1">
-        <v>2.8125000000000001E-2</v>
+        <v>5.6250000000000001E-2</v>
       </c>
       <c r="I31" s="1">
-        <v>2.9166666666666698E-2</v>
-      </c>
-      <c r="J31" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K31" s="2">
-        <v>2</v>
-      </c>
-      <c r="L31" s="2">
-        <v>41</v>
-      </c>
+        <v>5.8333333333333397E-2</v>
+      </c>
+      <c r="J31" s="10"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
       <c r="M31" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="N31" s="1">
         <v>2.8125000000000001E-2</v>
@@ -2418,8 +2434,7 @@
     </row>
     <row r="32" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
-        <f t="shared" si="0"/>
-        <v>45402</v>
+        <v>45359</v>
       </c>
       <c r="B32" s="1">
         <v>2.9166666666666698E-2</v>
@@ -2427,30 +2442,31 @@
       <c r="C32" s="1">
         <v>3.0208333333333399E-2</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="D32" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2">
+        <v>7</v>
+      </c>
+      <c r="F32" s="2">
+        <v>19</v>
+      </c>
       <c r="G32" s="15">
-        <v>45359</v>
+        <f t="shared" si="0"/>
+        <v>45402</v>
       </c>
       <c r="H32" s="1">
-        <v>2.9166666666666698E-2</v>
+        <v>5.83333333333333E-2</v>
       </c>
       <c r="I32" s="1">
-        <v>3.0208333333333399E-2</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K32" s="2">
-        <v>7</v>
-      </c>
-      <c r="L32" s="2">
-        <v>19</v>
-      </c>
+        <v>6.0416666666666702E-2</v>
+      </c>
+      <c r="J32" s="10"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
       <c r="M32" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45407</v>
+        <v>45408</v>
       </c>
       <c r="N32" s="1">
         <v>2.9166666666666698E-2</v>
@@ -2464,8 +2480,7 @@
     </row>
     <row r="33" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
-        <f t="shared" si="0"/>
-        <v>45403</v>
+        <v>45360</v>
       </c>
       <c r="B33" s="1">
         <v>3.0208333333333299E-2</v>
@@ -2473,30 +2488,31 @@
       <c r="C33" s="1">
         <v>3.125E-2</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="D33" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>37</v>
+      </c>
       <c r="G33" s="15">
-        <v>45360</v>
+        <f t="shared" si="0"/>
+        <v>45403</v>
       </c>
       <c r="H33" s="1">
-        <v>3.0208333333333299E-2</v>
+        <v>6.0416666666666702E-2</v>
       </c>
       <c r="I33" s="1">
-        <v>3.125E-2</v>
-      </c>
-      <c r="J33" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K33" s="2">
-        <v>0</v>
-      </c>
-      <c r="L33" s="2">
-        <v>37</v>
-      </c>
+        <v>6.2500000000000097E-2</v>
+      </c>
+      <c r="J33" s="10"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
       <c r="M33" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45408</v>
+        <v>45409</v>
       </c>
       <c r="N33" s="1">
         <v>3.0208333333333299E-2</v>
@@ -2510,8 +2526,7 @@
     </row>
     <row r="34" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
-        <f t="shared" si="0"/>
-        <v>45404</v>
+        <v>45361</v>
       </c>
       <c r="B34" s="1">
         <v>3.125E-2</v>
@@ -2519,30 +2534,31 @@
       <c r="C34" s="1">
         <v>3.2291666666666698E-2</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="D34" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2">
+        <v>3</v>
+      </c>
+      <c r="F34" s="2">
+        <v>14</v>
+      </c>
       <c r="G34" s="15">
-        <v>45361</v>
+        <f t="shared" si="0"/>
+        <v>45404</v>
       </c>
       <c r="H34" s="1">
-        <v>3.125E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="I34" s="1">
-        <v>3.2291666666666698E-2</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K34" s="2">
-        <v>3</v>
-      </c>
-      <c r="L34" s="2">
-        <v>14</v>
-      </c>
+        <v>6.4583333333333395E-2</v>
+      </c>
+      <c r="J34" s="10"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
       <c r="M34" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45409</v>
+        <v>45410</v>
       </c>
       <c r="N34" s="1">
         <v>3.125E-2</v>
@@ -2556,8 +2572,7 @@
     </row>
     <row r="35" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
-        <f t="shared" si="0"/>
-        <v>45405</v>
+        <v>45362</v>
       </c>
       <c r="B35" s="1">
         <v>3.2291666666666698E-2</v>
@@ -2565,30 +2580,31 @@
       <c r="C35" s="1">
         <v>3.3333333333333402E-2</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="D35" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="2">
+        <v>3</v>
+      </c>
+      <c r="F35" s="2">
+        <v>20</v>
+      </c>
       <c r="G35" s="15">
-        <v>45362</v>
+        <f t="shared" si="0"/>
+        <v>45405</v>
       </c>
       <c r="H35" s="1">
-        <v>3.2291666666666698E-2</v>
+        <v>6.4583333333333298E-2</v>
       </c>
       <c r="I35" s="1">
-        <v>3.3333333333333402E-2</v>
-      </c>
-      <c r="J35" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K35" s="2">
-        <v>3</v>
-      </c>
-      <c r="L35" s="2">
-        <v>20</v>
-      </c>
+        <v>6.6666666666666693E-2</v>
+      </c>
+      <c r="J35" s="10"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
       <c r="M35" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45410</v>
+        <v>45411</v>
       </c>
       <c r="N35" s="1">
         <v>3.2291666666666698E-2</v>
@@ -2602,8 +2618,7 @@
     </row>
     <row r="36" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
-        <f t="shared" si="0"/>
-        <v>45406</v>
+        <v>45363</v>
       </c>
       <c r="B36" s="1">
         <v>3.3333333333333298E-2</v>
@@ -2611,30 +2626,31 @@
       <c r="C36" s="1">
         <v>3.4375000000000003E-2</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="D36" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="2">
+        <v>4</v>
+      </c>
+      <c r="F36" s="2">
+        <v>37</v>
+      </c>
       <c r="G36" s="15">
-        <v>45363</v>
+        <f t="shared" si="0"/>
+        <v>45406</v>
       </c>
       <c r="H36" s="1">
-        <v>3.3333333333333298E-2</v>
+        <v>6.6666666666666693E-2</v>
       </c>
       <c r="I36" s="1">
-        <v>3.4375000000000003E-2</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K36" s="2">
-        <v>4</v>
-      </c>
-      <c r="L36" s="2">
-        <v>37</v>
-      </c>
+        <v>6.8750000000000103E-2</v>
+      </c>
+      <c r="J36" s="10"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
       <c r="M36" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="N36" s="1">
         <v>3.3333333333333298E-2</v>
@@ -2648,8 +2664,7 @@
     </row>
     <row r="37" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
-        <f t="shared" si="0"/>
-        <v>45407</v>
+        <v>45364</v>
       </c>
       <c r="B37" s="1">
         <v>3.4375000000000003E-2</v>
@@ -2657,30 +2672,31 @@
       <c r="C37" s="1">
         <v>3.54166666666667E-2</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="D37" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2">
+        <v>4</v>
+      </c>
+      <c r="F37" s="2">
+        <v>24</v>
+      </c>
       <c r="G37" s="15">
-        <v>45364</v>
+        <f t="shared" si="0"/>
+        <v>45407</v>
       </c>
       <c r="H37" s="1">
-        <v>3.4375000000000003E-2</v>
+        <v>6.8750000000000006E-2</v>
       </c>
       <c r="I37" s="1">
-        <v>3.54166666666667E-2</v>
-      </c>
-      <c r="J37" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K37" s="2">
-        <v>4</v>
-      </c>
-      <c r="L37" s="2">
-        <v>24</v>
-      </c>
+        <v>7.0833333333333401E-2</v>
+      </c>
+      <c r="J37" s="10"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
       <c r="M37" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45412</v>
+        <v>45413</v>
       </c>
       <c r="N37" s="1">
         <v>3.4375000000000003E-2</v>
@@ -2694,8 +2710,7 @@
     </row>
     <row r="38" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
-        <f t="shared" si="0"/>
-        <v>45408</v>
+        <v>45365</v>
       </c>
       <c r="B38" s="1">
         <v>3.54166666666667E-2</v>
@@ -2703,30 +2718,31 @@
       <c r="C38" s="1">
         <v>3.6458333333333398E-2</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="D38" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>5</v>
+      </c>
       <c r="G38" s="15">
-        <v>45365</v>
+        <f t="shared" si="0"/>
+        <v>45408</v>
       </c>
       <c r="H38" s="1">
-        <v>3.54166666666667E-2</v>
+        <v>7.0833333333333304E-2</v>
       </c>
       <c r="I38" s="1">
-        <v>3.6458333333333398E-2</v>
-      </c>
-      <c r="J38" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K38" s="2">
-        <v>2</v>
-      </c>
-      <c r="L38" s="2">
-        <v>5</v>
-      </c>
+        <v>7.2916666666666796E-2</v>
+      </c>
+      <c r="J38" s="10"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
       <c r="M38" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45413</v>
+        <v>45414</v>
       </c>
       <c r="N38" s="1">
         <v>3.54166666666667E-2</v>
@@ -2740,8 +2756,7 @@
     </row>
     <row r="39" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
-        <f t="shared" si="0"/>
-        <v>45409</v>
+        <v>45366</v>
       </c>
       <c r="B39" s="1">
         <v>3.6458333333333301E-2</v>
@@ -2749,30 +2764,31 @@
       <c r="C39" s="1">
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="D39" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2">
+        <v>4</v>
+      </c>
+      <c r="F39" s="2">
+        <v>16</v>
+      </c>
       <c r="G39" s="15">
-        <v>45366</v>
+        <f t="shared" si="0"/>
+        <v>45409</v>
       </c>
       <c r="H39" s="1">
-        <v>3.6458333333333301E-2</v>
+        <v>7.2916666666666699E-2</v>
       </c>
       <c r="I39" s="1">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="J39" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K39" s="2">
-        <v>4</v>
-      </c>
-      <c r="L39" s="2">
-        <v>16</v>
-      </c>
+        <v>7.5000000000000094E-2</v>
+      </c>
+      <c r="J39" s="10"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
       <c r="M39" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="N39" s="1">
         <v>3.6458333333333301E-2</v>
@@ -2786,8 +2802,7 @@
     </row>
     <row r="40" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
-        <f t="shared" si="0"/>
-        <v>45410</v>
+        <v>45367</v>
       </c>
       <c r="B40" s="1">
         <v>3.7499999999999999E-2</v>
@@ -2795,30 +2810,31 @@
       <c r="C40" s="1">
         <v>3.8541666666666703E-2</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+      <c r="D40" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="2">
+        <v>4</v>
+      </c>
+      <c r="F40" s="2">
+        <v>58</v>
+      </c>
       <c r="G40" s="15">
-        <v>45367</v>
+        <f t="shared" si="0"/>
+        <v>45410</v>
       </c>
       <c r="H40" s="1">
-        <v>3.7499999999999999E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="I40" s="1">
-        <v>3.8541666666666703E-2</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K40" s="2">
-        <v>4</v>
-      </c>
-      <c r="L40" s="2">
-        <v>58</v>
-      </c>
+        <v>7.7083333333333406E-2</v>
+      </c>
+      <c r="J40" s="10"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
       <c r="M40" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45415</v>
+        <v>45416</v>
       </c>
       <c r="N40" s="1">
         <v>3.7499999999999999E-2</v>
@@ -2832,8 +2848,8 @@
     </row>
     <row r="41" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
-        <f t="shared" si="0"/>
-        <v>45411</v>
+        <f ca="1">TODAY()</f>
+        <v>45380</v>
       </c>
       <c r="B41" s="1">
         <v>3.8541666666666703E-2</v>
@@ -2845,21 +2861,21 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="15">
-        <f ca="1">TODAY()</f>
-        <v>45379</v>
+        <f t="shared" si="0"/>
+        <v>45411</v>
       </c>
       <c r="H41" s="1">
-        <v>3.8541666666666703E-2</v>
+        <v>7.7083333333333295E-2</v>
       </c>
       <c r="I41" s="1">
-        <v>3.9583333333333401E-2</v>
+        <v>7.9166666666666802E-2</v>
       </c>
       <c r="J41" s="10"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45416</v>
+        <v>45417</v>
       </c>
       <c r="N41" s="1">
         <v>3.8541666666666703E-2</v>
@@ -2873,8 +2889,8 @@
     </row>
     <row r="42" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
-        <f t="shared" si="0"/>
-        <v>45412</v>
+        <f ca="1">A41+1</f>
+        <v>45381</v>
       </c>
       <c r="B42" s="1">
         <v>3.9583333333333297E-2</v>
@@ -2886,21 +2902,21 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="15">
-        <f ca="1">G41+1</f>
-        <v>45380</v>
+        <f t="shared" si="0"/>
+        <v>45412</v>
       </c>
       <c r="H42" s="1">
-        <v>3.9583333333333297E-2</v>
+        <v>7.9166666666666705E-2</v>
       </c>
       <c r="I42" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>8.12500000000001E-2</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45417</v>
+        <v>45418</v>
       </c>
       <c r="N42" s="1">
         <v>3.9583333333333297E-2</v>
@@ -2914,8 +2930,8 @@
     </row>
     <row r="43" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
-        <f t="shared" si="0"/>
-        <v>45413</v>
+        <f t="shared" ref="A43:A71" ca="1" si="2">A42+1</f>
+        <v>45382</v>
       </c>
       <c r="B43" s="1">
         <v>4.1666666666666664E-2</v>
@@ -2927,21 +2943,21 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="15">
-        <f t="shared" ref="G43:G71" ca="1" si="2">G42+1</f>
-        <v>45381</v>
+        <f t="shared" si="0"/>
+        <v>45413</v>
       </c>
       <c r="H43" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>8.1250000000000003E-2</v>
       </c>
       <c r="I43" s="1">
-        <v>4.5833333333333302E-2</v>
+        <v>8.3333333333333398E-2</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="N43" s="1">
         <v>4.1666666666666664E-2</v>
@@ -2955,8 +2971,8 @@
     </row>
     <row r="44" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
-        <f t="shared" si="0"/>
-        <v>45414</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45383</v>
       </c>
       <c r="B44" s="1">
         <v>4.5833333333333302E-2</v>
@@ -2968,21 +2984,21 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45382</v>
+        <f t="shared" si="0"/>
+        <v>45414</v>
       </c>
       <c r="H44" s="1">
-        <v>4.5833333333333302E-2</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="I44" s="1">
-        <v>5.00000000000001E-2</v>
+        <v>8.5416666666666793E-2</v>
       </c>
       <c r="J44" s="10"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45419</v>
+        <v>45420</v>
       </c>
       <c r="N44" s="1">
         <v>4.5833333333333302E-2</v>
@@ -2996,8 +3012,8 @@
     </row>
     <row r="45" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
-        <f t="shared" si="0"/>
-        <v>45415</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45384</v>
       </c>
       <c r="B45" s="1">
         <v>4.9999999999999899E-2</v>
@@ -3009,21 +3025,21 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45383</v>
+        <f t="shared" si="0"/>
+        <v>45415</v>
       </c>
       <c r="H45" s="1">
-        <v>4.9999999999999899E-2</v>
+        <v>8.5416666666666696E-2</v>
       </c>
       <c r="I45" s="1">
-        <v>5.4166666666666898E-2</v>
+        <v>8.7500000000000105E-2</v>
       </c>
       <c r="J45" s="10"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45420</v>
+        <v>45421</v>
       </c>
       <c r="N45" s="1">
         <v>4.9999999999999899E-2</v>
@@ -3037,8 +3053,8 @@
     </row>
     <row r="46" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
-        <f t="shared" si="0"/>
-        <v>45416</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45385</v>
       </c>
       <c r="B46" s="1">
         <v>5.4166666666666599E-2</v>
@@ -3050,21 +3066,21 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45384</v>
+        <f t="shared" si="0"/>
+        <v>45416</v>
       </c>
       <c r="H46" s="1">
-        <v>5.4166666666666599E-2</v>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="I46" s="1">
-        <v>5.8333333333333702E-2</v>
+        <v>8.9583333333333404E-2</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
       <c r="M46" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45421</v>
+        <v>45422</v>
       </c>
       <c r="N46" s="1">
         <v>5.4166666666666599E-2</v>
@@ -3078,8 +3094,8 @@
     </row>
     <row r="47" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
-        <f t="shared" si="0"/>
-        <v>45417</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45386</v>
       </c>
       <c r="B47" s="1">
         <v>5.83333333333333E-2</v>
@@ -3091,21 +3107,21 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45385</v>
+        <f t="shared" si="0"/>
+        <v>45417</v>
       </c>
       <c r="H47" s="1">
-        <v>5.83333333333333E-2</v>
+        <v>8.9583333333333307E-2</v>
       </c>
       <c r="I47" s="1">
-        <v>6.25000000000005E-2</v>
+        <v>9.1666666666666799E-2</v>
       </c>
       <c r="J47" s="10"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
       <c r="M47" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45422</v>
+        <v>45423</v>
       </c>
       <c r="N47" s="1">
         <v>5.83333333333333E-2</v>
@@ -3119,8 +3135,8 @@
     </row>
     <row r="48" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
-        <f t="shared" si="0"/>
-        <v>45418</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45387</v>
       </c>
       <c r="B48" s="1">
         <v>6.2499999999999903E-2</v>
@@ -3132,21 +3148,21 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45386</v>
+        <f t="shared" si="0"/>
+        <v>45418</v>
       </c>
       <c r="H48" s="1">
-        <v>6.2499999999999903E-2</v>
+        <v>9.1666666666666702E-2</v>
       </c>
       <c r="I48" s="1">
-        <v>6.6666666666667304E-2</v>
+        <v>9.3750000000000097E-2</v>
       </c>
       <c r="J48" s="10"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45423</v>
+        <v>45424</v>
       </c>
       <c r="N48" s="1">
         <v>6.2499999999999903E-2</v>
@@ -3160,8 +3176,8 @@
     </row>
     <row r="49" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
-        <f t="shared" si="0"/>
-        <v>45419</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45388</v>
       </c>
       <c r="B49" s="1">
         <v>6.6666666666666499E-2</v>
@@ -3173,21 +3189,21 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45387</v>
+        <f t="shared" si="0"/>
+        <v>45419</v>
       </c>
       <c r="H49" s="1">
-        <v>6.6666666666666499E-2</v>
+        <v>9.375E-2</v>
       </c>
       <c r="I49" s="1">
-        <v>7.0833333333334095E-2</v>
+        <v>9.5833333333333506E-2</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
       <c r="M49" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45424</v>
+        <v>45425</v>
       </c>
       <c r="N49" s="1">
         <v>6.6666666666666499E-2</v>
@@ -3201,8 +3217,8 @@
     </row>
     <row r="50" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
-        <f t="shared" si="0"/>
-        <v>45420</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45389</v>
       </c>
       <c r="B50" s="1">
         <v>7.0833333333333207E-2</v>
@@ -3214,21 +3230,21 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45388</v>
+        <f t="shared" si="0"/>
+        <v>45420</v>
       </c>
       <c r="H50" s="1">
-        <v>7.0833333333333207E-2</v>
+        <v>9.5833333333333298E-2</v>
       </c>
       <c r="I50" s="1">
-        <v>7.5000000000000899E-2</v>
+        <v>9.7916666666666805E-2</v>
       </c>
       <c r="J50" s="10"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45425</v>
+        <v>45426</v>
       </c>
       <c r="N50" s="1">
         <v>7.0833333333333207E-2</v>
@@ -3242,8 +3258,8 @@
     </row>
     <row r="51" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
-        <f t="shared" si="0"/>
-        <v>45421</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45390</v>
       </c>
       <c r="B51" s="1">
         <v>7.4999999999999803E-2</v>
@@ -3255,21 +3271,21 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45389</v>
+        <f t="shared" si="0"/>
+        <v>45421</v>
       </c>
       <c r="H51" s="1">
-        <v>7.4999999999999803E-2</v>
+        <v>9.7916666666666693E-2</v>
       </c>
       <c r="I51" s="1">
-        <v>7.9166666666667704E-2</v>
+        <v>0.1</v>
       </c>
       <c r="J51" s="10"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
       <c r="M51" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45426</v>
+        <v>45427</v>
       </c>
       <c r="N51" s="1">
         <v>7.4999999999999803E-2</v>
@@ -3283,8 +3299,8 @@
     </row>
     <row r="52" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
-        <f t="shared" si="0"/>
-        <v>45422</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45391</v>
       </c>
       <c r="B52" s="1">
         <v>7.9166666666666399E-2</v>
@@ -3296,21 +3312,21 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45390</v>
+        <f t="shared" si="0"/>
+        <v>45422</v>
       </c>
       <c r="H52" s="1">
-        <v>7.9166666666666399E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I52" s="1">
-        <v>8.3333333333334494E-2</v>
+        <v>0.102083333333333</v>
       </c>
       <c r="J52" s="10"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45427</v>
+        <v>45428</v>
       </c>
       <c r="N52" s="1">
         <v>7.9166666666666399E-2</v>
@@ -3324,8 +3340,8 @@
     </row>
     <row r="53" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
-        <f t="shared" si="0"/>
-        <v>45423</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45392</v>
       </c>
       <c r="B53" s="1">
         <v>8.3333333333333107E-2</v>
@@ -3337,21 +3353,21 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45391</v>
+        <f t="shared" si="0"/>
+        <v>45423</v>
       </c>
       <c r="H53" s="1">
-        <v>8.3333333333333107E-2</v>
+        <v>0.102083333333333</v>
       </c>
       <c r="I53" s="1">
-        <v>9.0277777777777776E-2</v>
+        <v>0.10416666666666601</v>
       </c>
       <c r="J53" s="10"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
       <c r="M53" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45428</v>
+        <v>45429</v>
       </c>
       <c r="N53" s="1">
         <v>8.3333333333333107E-2</v>
@@ -3365,8 +3381,8 @@
     </row>
     <row r="54" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
-        <f t="shared" si="0"/>
-        <v>45424</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45393</v>
       </c>
       <c r="B54" s="1">
         <v>9.0277777777777776E-2</v>
@@ -3378,21 +3394,21 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45392</v>
+        <f t="shared" si="0"/>
+        <v>45424</v>
       </c>
       <c r="H54" s="1">
-        <v>9.0277777777777776E-2</v>
+        <v>0.104166666666667</v>
       </c>
       <c r="I54" s="1">
-        <v>9.7222222222222224E-2</v>
+        <v>0.10625</v>
       </c>
       <c r="J54" s="10"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
       <c r="M54" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45429</v>
+        <v>45430</v>
       </c>
       <c r="N54" s="1">
         <v>9.0277777777777776E-2</v>
@@ -3406,8 +3422,8 @@
     </row>
     <row r="55" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
-        <f t="shared" si="0"/>
-        <v>45425</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45394</v>
       </c>
       <c r="B55" s="1">
         <v>9.7222222222222404E-2</v>
@@ -3419,21 +3435,21 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45393</v>
+        <f t="shared" si="0"/>
+        <v>45425</v>
       </c>
       <c r="H55" s="1">
-        <v>9.7222222222222404E-2</v>
+        <v>0.10625</v>
       </c>
       <c r="I55" s="1">
-        <v>0.104166666666667</v>
+        <v>0.108333333333333</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
       <c r="M55" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45430</v>
+        <v>45431</v>
       </c>
       <c r="N55" s="1">
         <v>9.7222222222222404E-2</v>
@@ -3447,8 +3463,8 @@
     </row>
     <row r="56" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
-        <f t="shared" si="0"/>
-        <v>45426</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45395</v>
       </c>
       <c r="B56" s="1">
         <v>0.104166666666667</v>
@@ -3460,21 +3476,21 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45394</v>
+        <f t="shared" si="0"/>
+        <v>45426</v>
       </c>
       <c r="H56" s="1">
-        <v>0.104166666666667</v>
+        <v>0.108333333333333</v>
       </c>
       <c r="I56" s="1">
-        <v>0.11111111111111099</v>
+        <v>0.110416666666667</v>
       </c>
       <c r="J56" s="10"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45431</v>
+        <v>45432</v>
       </c>
       <c r="N56" s="1">
         <v>0.104166666666667</v>
@@ -3488,8 +3504,8 @@
     </row>
     <row r="57" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
-        <f t="shared" si="0"/>
-        <v>45427</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45396</v>
       </c>
       <c r="B57" s="1">
         <v>0.11111111111111199</v>
@@ -3501,21 +3517,21 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45395</v>
+        <f t="shared" si="0"/>
+        <v>45427</v>
       </c>
       <c r="H57" s="1">
-        <v>0.11111111111111199</v>
+        <v>0.110416666666667</v>
       </c>
       <c r="I57" s="1">
-        <v>0.118055555555556</v>
+        <v>0.1125</v>
       </c>
       <c r="J57" s="10"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45432</v>
+        <v>45433</v>
       </c>
       <c r="N57" s="1">
         <v>0.11111111111111199</v>
@@ -3529,8 +3545,8 @@
     </row>
     <row r="58" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
-        <f t="shared" si="0"/>
-        <v>45428</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45397</v>
       </c>
       <c r="B58" s="1">
         <v>0.118055555555556</v>
@@ -3542,21 +3558,21 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45396</v>
+        <f t="shared" si="0"/>
+        <v>45428</v>
       </c>
       <c r="H58" s="1">
-        <v>0.118055555555556</v>
+        <v>0.1125</v>
       </c>
       <c r="I58" s="1">
-        <v>0.125</v>
+        <v>0.114583333333333</v>
       </c>
       <c r="J58" s="10"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45433</v>
+        <v>45434</v>
       </c>
       <c r="N58" s="1">
         <v>0.118055555555556</v>
@@ -3570,8 +3586,8 @@
     </row>
     <row r="59" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
-        <f t="shared" si="0"/>
-        <v>45429</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45398</v>
       </c>
       <c r="B59" s="1">
         <v>0.125000000000001</v>
@@ -3583,21 +3599,21 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45397</v>
+        <f t="shared" si="0"/>
+        <v>45429</v>
       </c>
       <c r="H59" s="1">
-        <v>0.125000000000001</v>
+        <v>0.114583333333333</v>
       </c>
       <c r="I59" s="1">
-        <v>0.131944444444444</v>
+        <v>0.116666666666667</v>
       </c>
       <c r="J59" s="10"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45434</v>
+        <v>45435</v>
       </c>
       <c r="N59" s="1">
         <v>0.125000000000001</v>
@@ -3611,8 +3627,8 @@
     </row>
     <row r="60" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
-        <f t="shared" si="0"/>
-        <v>45430</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45399</v>
       </c>
       <c r="B60" s="1">
         <v>0.131944444444446</v>
@@ -3624,21 +3640,21 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45398</v>
+        <f t="shared" si="0"/>
+        <v>45430</v>
       </c>
       <c r="H60" s="1">
-        <v>0.131944444444446</v>
+        <v>0.116666666666667</v>
       </c>
       <c r="I60" s="1">
-        <v>0.13888888888888901</v>
+        <v>0.11874999999999999</v>
       </c>
       <c r="J60" s="10"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
       <c r="M60" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45435</v>
+        <v>45436</v>
       </c>
       <c r="N60" s="1">
         <v>0.131944444444446</v>
@@ -3652,8 +3668,8 @@
     </row>
     <row r="61" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
-        <f t="shared" si="0"/>
-        <v>45431</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45400</v>
       </c>
       <c r="B61" s="1">
         <v>0.138888888888891</v>
@@ -3665,21 +3681,21 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45399</v>
+        <f t="shared" si="0"/>
+        <v>45431</v>
       </c>
       <c r="H61" s="1">
-        <v>0.138888888888891</v>
+        <v>0.11874999999999999</v>
       </c>
       <c r="I61" s="1">
-        <v>0.14583333333333301</v>
+        <v>0.120833333333333</v>
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
       <c r="M61" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45436</v>
+        <v>45437</v>
       </c>
       <c r="N61" s="1">
         <v>0.138888888888891</v>
@@ -3693,8 +3709,8 @@
     </row>
     <row r="62" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
-        <f t="shared" si="0"/>
-        <v>45432</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45401</v>
       </c>
       <c r="B62" s="1">
         <v>0.14583333333333501</v>
@@ -3706,14 +3722,14 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45400</v>
+        <f t="shared" si="0"/>
+        <v>45432</v>
       </c>
       <c r="H62" s="1">
-        <v>0.14583333333333501</v>
+        <v>0.120833333333333</v>
       </c>
       <c r="I62" s="1">
-        <v>0.15277777777777801</v>
+        <v>0.12291666666666699</v>
       </c>
       <c r="J62" s="10"/>
       <c r="K62" s="2"/>
@@ -3727,8 +3743,8 @@
     </row>
     <row r="63" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
-        <f t="shared" si="0"/>
-        <v>45433</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45402</v>
       </c>
       <c r="B63" s="1">
         <v>0.15277777777778001</v>
@@ -3740,14 +3756,14 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45401</v>
+        <f t="shared" si="0"/>
+        <v>45433</v>
       </c>
       <c r="H63" s="1">
-        <v>0.15277777777778001</v>
+        <v>0.12291666666666699</v>
       </c>
       <c r="I63" s="1">
-        <v>0.15972222222222199</v>
+        <v>0.125</v>
       </c>
       <c r="J63" s="10"/>
       <c r="K63" s="2"/>
@@ -3761,8 +3777,8 @@
     </row>
     <row r="64" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
-        <f t="shared" si="0"/>
-        <v>45434</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45403</v>
       </c>
       <c r="B64" s="1">
         <v>0.15972222222222399</v>
@@ -3774,14 +3790,14 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45402</v>
+        <f t="shared" si="0"/>
+        <v>45434</v>
       </c>
       <c r="H64" s="1">
-        <v>0.15972222222222399</v>
+        <v>0.125</v>
       </c>
       <c r="I64" s="1">
-        <v>0.16666666666666699</v>
+        <v>0.12708333333333299</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="2"/>
@@ -3795,8 +3811,8 @@
     </row>
     <row r="65" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
-        <f t="shared" si="0"/>
-        <v>45435</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45404</v>
       </c>
       <c r="B65" s="1">
         <v>0.16666666666666899</v>
@@ -3808,14 +3824,14 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45403</v>
+        <f t="shared" si="0"/>
+        <v>45435</v>
       </c>
       <c r="H65" s="1">
-        <v>0.16666666666666899</v>
+        <v>0.12708333333333299</v>
       </c>
       <c r="I65" s="1">
-        <v>0.17361111111111099</v>
+        <v>0.12916666666666701</v>
       </c>
       <c r="J65" s="10"/>
       <c r="K65" s="2"/>
@@ -3829,8 +3845,8 @@
     </row>
     <row r="66" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
-        <f t="shared" si="0"/>
-        <v>45436</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45405</v>
       </c>
       <c r="B66" s="1">
         <v>0.17361111111111399</v>
@@ -3842,14 +3858,14 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45404</v>
+        <f t="shared" si="0"/>
+        <v>45436</v>
       </c>
       <c r="H66" s="1">
-        <v>0.17361111111111399</v>
+        <v>0.12916666666666701</v>
       </c>
       <c r="I66" s="1">
-        <v>0.180555555555556</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="J66" s="10"/>
       <c r="K66" s="2"/>
@@ -3863,8 +3879,8 @@
     </row>
     <row r="67" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
-        <f t="shared" si="0"/>
-        <v>45437</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45406</v>
       </c>
       <c r="B67" s="1">
         <v>0.18055555555555899</v>
@@ -3876,14 +3892,14 @@
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45405</v>
+        <f t="shared" si="0"/>
+        <v>45437</v>
       </c>
       <c r="H67" s="1">
-        <v>0.18055555555555899</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="I67" s="1">
-        <v>0.1875</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="2"/>
@@ -3897,8 +3913,8 @@
     </row>
     <row r="68" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
-        <f t="shared" si="0"/>
-        <v>45438</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45407</v>
       </c>
       <c r="B68" s="1">
         <v>0.187500000000003</v>
@@ -3910,14 +3926,14 @@
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45406</v>
+        <f t="shared" si="0"/>
+        <v>45438</v>
       </c>
       <c r="H68" s="1">
-        <v>0.187500000000003</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="I68" s="1">
-        <v>0.194444444444445</v>
+        <v>0.13541666666666699</v>
       </c>
       <c r="J68" s="10"/>
       <c r="K68" s="2"/>
@@ -3931,8 +3947,8 @@
     </row>
     <row r="69" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
-        <f t="shared" si="0"/>
-        <v>45439</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45408</v>
       </c>
       <c r="B69" s="1">
         <v>0.194444444444448</v>
@@ -3944,14 +3960,14 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45407</v>
+        <f t="shared" si="0"/>
+        <v>45439</v>
       </c>
       <c r="H69" s="1">
-        <v>0.194444444444448</v>
+        <v>0.13541666666666699</v>
       </c>
       <c r="I69" s="1">
-        <v>0.20138888888888901</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="J69" s="10"/>
       <c r="K69" s="2"/>
@@ -3965,8 +3981,8 @@
     </row>
     <row r="70" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
-        <f t="shared" ref="A70:A71" si="3">A69+1</f>
-        <v>45440</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45409</v>
       </c>
       <c r="B70" s="1">
         <v>0.201388888888892</v>
@@ -3978,14 +3994,14 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45408</v>
+        <f t="shared" ref="G70:G71" si="3">G69+1</f>
+        <v>45440</v>
       </c>
       <c r="H70" s="1">
-        <v>0.201388888888892</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="I70" s="1">
-        <v>0.20833333333333401</v>
+        <v>0.139583333333333</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="2"/>
@@ -3999,8 +4015,8 @@
     </row>
     <row r="71" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
-        <f t="shared" si="3"/>
-        <v>45441</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45410</v>
       </c>
       <c r="B71" s="1">
         <v>0.20833333333333701</v>
@@ -4012,14 +4028,14 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>45409</v>
+        <f t="shared" si="3"/>
+        <v>45441</v>
       </c>
       <c r="H71" s="1">
-        <v>0.20833333333333701</v>
+        <v>0.139583333333333</v>
       </c>
       <c r="I71" s="1">
-        <v>0.21527777777777801</v>
+        <v>0.141666666666667</v>
       </c>
       <c r="J71" s="10"/>
       <c r="K71" s="2"/>
@@ -4035,8 +4051,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="M1:P2"/>
+    <mergeCell ref="G1:J2"/>
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="G1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Attempt to Submit Form failed 1
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f7c3dc73fd6fbfd/Desktop/dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{7440CBCE-681D-46D5-A872-89873CD1139C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4C2FEF2-E1AE-43B3-BF2F-12BC74F277A1}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{7440CBCE-681D-46D5-A872-89873CD1139C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{609353C9-196D-441C-8448-8B456E313090}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -568,6 +568,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A42150A-74BB-4659-8BE3-C38AE4DF6F2F}" name="Table22" displayName="Table22" ref="A3:D71" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A3:D71" xr:uid="{9A42150A-74BB-4659-8BE3-C38AE4DF6F2F}"/>
@@ -873,7 +877,7 @@
   <dimension ref="A1:R72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -1997,7 +2001,9 @@
       <c r="I22" s="1">
         <v>3.9583333333333401E-2</v>
       </c>
-      <c r="J22" s="10"/>
+      <c r="J22" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="K22" s="2">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
aDDing Right bAR TO ISSUES
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0F03DF-DAB1-4554-AC1C-05BB1C1999F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F33212-E06D-4F9B-9E74-2185533A1E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -269,6 +269,9 @@
     <xf numFmtId="168" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -278,9 +281,6 @@
     <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent4" xfId="2" builtinId="41"/>
@@ -288,6 +288,22 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -385,7 +401,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -402,8 +417,56 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -452,70 +515,6 @@
       </font>
       <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -607,12 +606,27 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -628,56 +642,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -758,6 +724,40 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -793,49 +793,49 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A42150A-74BB-4659-8BE3-C38AE4DF6F2F}" name="Table1" displayName="Table1" ref="A3:D71" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A3:D71" xr:uid="{9A42150A-74BB-4659-8BE3-C38AE4DF6F2F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E47A06B2-66D0-4A3B-94F5-F413F13FA3D5}" name="Date" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{263AAFE7-CED9-4BC8-BDF4-682077A1A32F}" name="FROM" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{85D092AB-1643-4507-9EDE-D374E629A267}" name="TO" dataDxfId="21" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{0B7EAA86-C05E-4B44-925F-0BC8C8A53CE4}" name="CHECK" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{E47A06B2-66D0-4A3B-94F5-F413F13FA3D5}" name="Date" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{263AAFE7-CED9-4BC8-BDF4-682077A1A32F}" name="FROM" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{85D092AB-1643-4507-9EDE-D374E629A267}" name="TO" dataDxfId="19" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{0B7EAA86-C05E-4B44-925F-0BC8C8A53CE4}" name="CHECK" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C40EC8C8-11F4-4B98-8E22-DE0BEA09C108}" name="Table3" displayName="Table3" ref="M3:P71" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C40EC8C8-11F4-4B98-8E22-DE0BEA09C108}" name="Table3" displayName="Table3" ref="M3:P71" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="M3:P71" xr:uid="{C40EC8C8-11F4-4B98-8E22-DE0BEA09C108}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9034DB75-A35D-40DA-9B02-E245B29B906D}" name="Date" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{9D116230-888C-4DC0-9632-4961EC573E06}" name="FROM" dataDxfId="7" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{A59F171F-3DF7-49EB-BCD6-30A73E3AE642}" name="TO" dataDxfId="17" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{5F9CFA76-FB56-45C5-85EA-F0A0C4814ED9}" name="CHECK" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{9034DB75-A35D-40DA-9B02-E245B29B906D}" name="Date" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{9D116230-888C-4DC0-9632-4961EC573E06}" name="FROM" dataDxfId="14" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{A59F171F-3DF7-49EB-BCD6-30A73E3AE642}" name="TO" dataDxfId="13" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{5F9CFA76-FB56-45C5-85EA-F0A0C4814ED9}" name="CHECK" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E2833A92-15F0-45DF-8153-A7603B424774}" name="Table2" displayName="Table2" ref="G3:J71" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E2833A92-15F0-45DF-8153-A7603B424774}" name="Table2" displayName="Table2" ref="G3:J71" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="G3:J71" xr:uid="{E2833A92-15F0-45DF-8153-A7603B424774}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F939511D-5FD6-4F93-B2DB-3FBFE1C3FCD5}" name="Date" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{1AE9D2F2-DAC2-4413-9B1B-4723A3CDD042}" name="FROM" dataDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{AEE26E09-6685-4A24-9E50-62100CDCD428}" name="TO" dataDxfId="13" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{117B0C20-5798-4D67-8692-5742681B2FB9}" name="CHECK" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{F939511D-5FD6-4F93-B2DB-3FBFE1C3FCD5}" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{1AE9D2F2-DAC2-4413-9B1B-4723A3CDD042}" name="FROM" dataDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{AEE26E09-6685-4A24-9E50-62100CDCD428}" name="TO" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{117B0C20-5798-4D67-8692-5742681B2FB9}" name="CHECK" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6CC927E-383C-4EF3-9AED-51EAE20B008F}" name="Table13" displayName="Table13" ref="S3:V71" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6CC927E-383C-4EF3-9AED-51EAE20B008F}" name="Table13" displayName="Table13" ref="S3:V71" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="S3:V71" xr:uid="{A6CC927E-383C-4EF3-9AED-51EAE20B008F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8F1B30E1-E6FB-4D36-AC9C-A359A0E5858E}" name="Date" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{E0AC3131-F12B-46C3-B027-4C11D754863C}" name="FROM" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{1C4330AB-234C-44BD-8D07-29F14CFFC28D}" name="TO" dataDxfId="0" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{B5C0519C-703D-4190-83FB-B1375C40392B}" name="CHECK" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{8F1B30E1-E6FB-4D36-AC9C-A359A0E5858E}" name="Date" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{E0AC3131-F12B-46C3-B027-4C11D754863C}" name="FROM" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{1C4330AB-234C-44BD-8D07-29F14CFFC28D}" name="TO" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{B5C0519C-703D-4190-83FB-B1375C40392B}" name="CHECK" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1106,9 +1106,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F4D59D-8EC0-4300-B06F-D1EA277B0BF1}">
   <dimension ref="A1:X72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V11" sqref="V11"/>
+      <selection pane="bottomLeft" activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -1135,48 +1135,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
       <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
       <c r="Q1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
       <c r="W1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1185,10 +1185,10 @@
       </c>
     </row>
     <row r="2" spans="1:24" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="6">
         <f>(E3+(F3/60))/60</f>
         <v>1.3583333333333334</v>
@@ -1197,10 +1197,10 @@
         <f>(E3+(F3/60))</f>
         <v>81.5</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
       <c r="K2" s="6">
         <f>(K3+(L3/60))/60</f>
         <v>0</v>
@@ -1209,10 +1209,10 @@
         <f>(K3+(L3/60))</f>
         <v>0</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
       <c r="Q2" s="6">
         <f>(Q3+(R3/60))/60</f>
         <v>0</v>
@@ -1221,10 +1221,10 @@
         <f>(Q3+(R3/60))</f>
         <v>0</v>
       </c>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
       <c r="W2" s="6">
         <f>(W3+(X3/60))/60</f>
         <v>0.26666666666666666</v>
@@ -1317,7 +1317,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="19">
+      <c r="A4" s="16">
         <v>45383</v>
       </c>
       <c r="B4" s="1">
@@ -1335,7 +1335,7 @@
       <c r="F4" s="2">
         <v>21</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="16">
         <v>45374</v>
       </c>
       <c r="H4" s="1">
@@ -1351,7 +1351,7 @@
       <c r="L4" s="2">
         <v>2</v>
       </c>
-      <c r="M4" s="19">
+      <c r="M4" s="16">
         <f ca="1">TODAY()</f>
         <v>45384</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="19">
+      <c r="S4" s="16">
         <v>45384</v>
       </c>
       <c r="T4" s="1">
@@ -1384,7 +1384,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19">
+      <c r="A5" s="16">
         <f>A4+1</f>
         <v>45384</v>
       </c>
@@ -1403,7 +1403,7 @@
       <c r="F5" s="2">
         <v>4</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="16">
         <f>G4+1</f>
         <v>45375</v>
       </c>
@@ -1420,7 +1420,7 @@
       <c r="L5" s="2">
         <v>48</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="16">
         <f ca="1">M4+1</f>
         <v>45385</v>
       </c>
@@ -1433,7 +1433,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="19">
+      <c r="S5" s="16">
         <f>S4+1</f>
         <v>45385</v>
       </c>
@@ -1454,7 +1454,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19">
+      <c r="A6" s="16">
         <f t="shared" ref="A6:A69" si="0">A5+1</f>
         <v>45385</v>
       </c>
@@ -1473,7 +1473,7 @@
       <c r="F6" s="2">
         <v>25</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="16">
         <f t="shared" ref="G6:G69" si="1">G5+1</f>
         <v>45376</v>
       </c>
@@ -1490,7 +1490,7 @@
       <c r="L6" s="2">
         <v>38</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="16">
         <f t="shared" ref="M6:M61" ca="1" si="2">M5+1</f>
         <v>45386</v>
       </c>
@@ -1503,7 +1503,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="19">
+      <c r="S6" s="16">
         <f t="shared" ref="S6:S69" si="3">S5+1</f>
         <v>45386</v>
       </c>
@@ -1524,7 +1524,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19">
+      <c r="A7" s="16">
         <f t="shared" si="0"/>
         <v>45386</v>
       </c>
@@ -1543,7 +1543,7 @@
       <c r="F7" s="2">
         <v>38</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="16">
         <f t="shared" si="1"/>
         <v>45377</v>
       </c>
@@ -1560,7 +1560,7 @@
       <c r="L7" s="2">
         <v>58</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45387</v>
       </c>
@@ -1573,7 +1573,7 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="19">
+      <c r="S7" s="16">
         <f t="shared" si="3"/>
         <v>45387</v>
       </c>
@@ -1594,7 +1594,7 @@
       </c>
     </row>
     <row r="8" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="19">
+      <c r="A8" s="16">
         <f t="shared" si="0"/>
         <v>45387</v>
       </c>
@@ -1613,7 +1613,7 @@
       <c r="F8" s="2">
         <v>41</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="16">
         <f t="shared" si="1"/>
         <v>45378</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="L8" s="2">
         <v>15</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45388</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="19">
+      <c r="S8" s="16">
         <f t="shared" si="3"/>
         <v>45388</v>
       </c>
@@ -1664,7 +1664,7 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="19">
+      <c r="A9" s="16">
         <f t="shared" si="0"/>
         <v>45388</v>
       </c>
@@ -1683,7 +1683,7 @@
       <c r="F9" s="2">
         <v>24</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="16">
         <f t="shared" si="1"/>
         <v>45379</v>
       </c>
@@ -1700,7 +1700,7 @@
       <c r="L9" s="2">
         <v>17</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45389</v>
       </c>
@@ -1713,7 +1713,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="19">
+      <c r="S9" s="16">
         <f t="shared" si="3"/>
         <v>45389</v>
       </c>
@@ -1734,7 +1734,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19">
+      <c r="A10" s="16">
         <f t="shared" si="0"/>
         <v>45389</v>
       </c>
@@ -1753,7 +1753,7 @@
       <c r="F10" s="2">
         <v>22</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="16">
         <f t="shared" si="1"/>
         <v>45380</v>
       </c>
@@ -1770,7 +1770,7 @@
       <c r="L10" s="2">
         <v>51</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45390</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="19">
+      <c r="S10" s="16">
         <f t="shared" si="3"/>
         <v>45390</v>
       </c>
@@ -1804,7 +1804,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19">
+      <c r="A11" s="16">
         <f t="shared" si="0"/>
         <v>45390</v>
       </c>
@@ -1823,7 +1823,7 @@
       <c r="F11" s="2">
         <v>49</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="16">
         <f t="shared" si="1"/>
         <v>45381</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="L11" s="2">
         <v>52</v>
       </c>
-      <c r="M11" s="19">
+      <c r="M11" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45391</v>
       </c>
@@ -1853,7 +1853,7 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="19">
+      <c r="S11" s="16">
         <f t="shared" si="3"/>
         <v>45391</v>
       </c>
@@ -1874,7 +1874,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19">
+      <c r="A12" s="16">
         <f t="shared" si="0"/>
         <v>45391</v>
       </c>
@@ -1893,7 +1893,7 @@
       <c r="F12" s="2">
         <v>15</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="16">
         <f t="shared" si="1"/>
         <v>45382</v>
       </c>
@@ -1910,7 +1910,7 @@
       <c r="L12" s="2">
         <v>17</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45392</v>
       </c>
@@ -1923,7 +1923,7 @@
       <c r="P12" s="9"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="19">
+      <c r="S12" s="16">
         <f t="shared" si="3"/>
         <v>45392</v>
       </c>
@@ -1942,7 +1942,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="19">
+      <c r="A13" s="16">
         <f t="shared" si="0"/>
         <v>45392</v>
       </c>
@@ -1961,7 +1961,7 @@
       <c r="F13" s="2">
         <v>13</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="16">
         <f t="shared" si="1"/>
         <v>45383</v>
       </c>
@@ -1978,7 +1978,7 @@
       <c r="L13" s="2">
         <v>58</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45393</v>
       </c>
@@ -1991,7 +1991,7 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="19">
+      <c r="S13" s="16">
         <f t="shared" si="3"/>
         <v>45393</v>
       </c>
@@ -2010,7 +2010,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="19">
+      <c r="A14" s="16">
         <f t="shared" si="0"/>
         <v>45393</v>
       </c>
@@ -2029,7 +2029,7 @@
       <c r="F14" s="2">
         <v>4</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="16">
         <f t="shared" si="1"/>
         <v>45384</v>
       </c>
@@ -2046,7 +2046,7 @@
       <c r="L14" s="2">
         <v>45</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45394</v>
       </c>
@@ -2059,7 +2059,7 @@
       <c r="P14" s="9"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="19">
+      <c r="S14" s="16">
         <f t="shared" si="3"/>
         <v>45394</v>
       </c>
@@ -2078,7 +2078,7 @@
       </c>
     </row>
     <row r="15" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19">
+      <c r="A15" s="16">
         <f t="shared" si="0"/>
         <v>45394</v>
       </c>
@@ -2097,7 +2097,7 @@
       <c r="F15" s="2">
         <v>25</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="16">
         <f t="shared" si="1"/>
         <v>45385</v>
       </c>
@@ -2114,7 +2114,7 @@
       <c r="L15" s="2">
         <v>40</v>
       </c>
-      <c r="M15" s="19">
+      <c r="M15" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45395</v>
       </c>
@@ -2127,7 +2127,7 @@
       <c r="P15" s="9"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="19">
+      <c r="S15" s="16">
         <f t="shared" si="3"/>
         <v>45395</v>
       </c>
@@ -2146,7 +2146,7 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="19">
+      <c r="A16" s="16">
         <f t="shared" si="0"/>
         <v>45395</v>
       </c>
@@ -2165,7 +2165,7 @@
       <c r="F16" s="2">
         <v>9</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="16">
         <f t="shared" si="1"/>
         <v>45386</v>
       </c>
@@ -2182,7 +2182,7 @@
       <c r="L16" s="2">
         <v>54</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45396</v>
       </c>
@@ -2195,7 +2195,7 @@
       <c r="P16" s="9"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="19">
+      <c r="S16" s="16">
         <f t="shared" si="3"/>
         <v>45396</v>
       </c>
@@ -2214,7 +2214,7 @@
       </c>
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19">
+      <c r="A17" s="16">
         <f t="shared" si="0"/>
         <v>45396</v>
       </c>
@@ -2233,7 +2233,7 @@
       <c r="F17" s="2">
         <v>20</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="16">
         <f t="shared" si="1"/>
         <v>45387</v>
       </c>
@@ -2250,7 +2250,7 @@
       <c r="L17" s="2">
         <v>32</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45397</v>
       </c>
@@ -2263,7 +2263,7 @@
       <c r="P17" s="9"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="19">
+      <c r="S17" s="16">
         <f t="shared" si="3"/>
         <v>45397</v>
       </c>
@@ -2282,7 +2282,7 @@
       </c>
     </row>
     <row r="18" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="19">
+      <c r="A18" s="16">
         <f t="shared" si="0"/>
         <v>45397</v>
       </c>
@@ -2301,7 +2301,7 @@
       <c r="F18" s="2">
         <v>34</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="16">
         <f t="shared" si="1"/>
         <v>45388</v>
       </c>
@@ -2318,7 +2318,7 @@
       <c r="L18" s="2">
         <v>57</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45398</v>
       </c>
@@ -2331,7 +2331,7 @@
       <c r="P18" s="9"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="19">
+      <c r="S18" s="16">
         <f t="shared" si="3"/>
         <v>45398</v>
       </c>
@@ -2350,7 +2350,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="19">
+      <c r="A19" s="16">
         <f t="shared" si="0"/>
         <v>45398</v>
       </c>
@@ -2369,7 +2369,7 @@
       <c r="F19" s="2">
         <v>27</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="16">
         <f t="shared" si="1"/>
         <v>45389</v>
       </c>
@@ -2386,7 +2386,7 @@
       <c r="L19" s="2">
         <v>52</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M19" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45399</v>
       </c>
@@ -2399,7 +2399,7 @@
       <c r="P19" s="9"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
-      <c r="S19" s="19">
+      <c r="S19" s="16">
         <f t="shared" si="3"/>
         <v>45399</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="X19" s="2"/>
     </row>
     <row r="20" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="19">
+      <c r="A20" s="16">
         <f t="shared" si="0"/>
         <v>45399</v>
       </c>
@@ -2433,7 +2433,7 @@
       <c r="F20" s="2">
         <v>39</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="16">
         <f t="shared" si="1"/>
         <v>45390</v>
       </c>
@@ -2450,7 +2450,7 @@
       <c r="L20" s="2">
         <v>0</v>
       </c>
-      <c r="M20" s="19">
+      <c r="M20" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45400</v>
       </c>
@@ -2463,7 +2463,7 @@
       <c r="P20" s="9"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
-      <c r="S20" s="19">
+      <c r="S20" s="16">
         <f t="shared" si="3"/>
         <v>45400</v>
       </c>
@@ -2478,7 +2478,7 @@
       <c r="X20" s="2"/>
     </row>
     <row r="21" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="19">
+      <c r="A21" s="16">
         <f t="shared" si="0"/>
         <v>45400</v>
       </c>
@@ -2497,7 +2497,7 @@
       <c r="F21" s="2">
         <v>17</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="16">
         <f t="shared" si="1"/>
         <v>45391</v>
       </c>
@@ -2514,7 +2514,7 @@
       <c r="L21" s="2">
         <v>55</v>
       </c>
-      <c r="M21" s="19">
+      <c r="M21" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45401</v>
       </c>
@@ -2527,7 +2527,7 @@
       <c r="P21" s="9"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
-      <c r="S21" s="19">
+      <c r="S21" s="16">
         <f t="shared" si="3"/>
         <v>45401</v>
       </c>
@@ -2542,7 +2542,7 @@
       <c r="X21" s="2"/>
     </row>
     <row r="22" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="19">
+      <c r="A22" s="16">
         <f t="shared" si="0"/>
         <v>45401</v>
       </c>
@@ -2561,7 +2561,7 @@
       <c r="F22" s="2">
         <v>27</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="16">
         <f t="shared" si="1"/>
         <v>45392</v>
       </c>
@@ -2578,7 +2578,7 @@
       <c r="L22" s="2">
         <v>43</v>
       </c>
-      <c r="M22" s="19">
+      <c r="M22" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45402</v>
       </c>
@@ -2591,7 +2591,7 @@
       <c r="P22" s="9"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
-      <c r="S22" s="19">
+      <c r="S22" s="16">
         <f t="shared" si="3"/>
         <v>45402</v>
       </c>
@@ -2606,7 +2606,7 @@
       <c r="X22" s="2"/>
     </row>
     <row r="23" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19">
+      <c r="A23" s="16">
         <f t="shared" si="0"/>
         <v>45402</v>
       </c>
@@ -2625,7 +2625,7 @@
       <c r="F23" s="2">
         <v>54</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="16">
         <f t="shared" si="1"/>
         <v>45393</v>
       </c>
@@ -2638,7 +2638,7 @@
       <c r="J23" s="9"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="19">
+      <c r="M23" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45403</v>
       </c>
@@ -2651,7 +2651,7 @@
       <c r="P23" s="9"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="19">
+      <c r="S23" s="16">
         <f t="shared" si="3"/>
         <v>45403</v>
       </c>
@@ -2666,7 +2666,7 @@
       <c r="X23" s="2"/>
     </row>
     <row r="24" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19">
+      <c r="A24" s="16">
         <f t="shared" si="0"/>
         <v>45403</v>
       </c>
@@ -2685,7 +2685,7 @@
       <c r="F24" s="2">
         <v>59</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="16">
         <f t="shared" si="1"/>
         <v>45394</v>
       </c>
@@ -2698,7 +2698,7 @@
       <c r="J24" s="9"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="19">
+      <c r="M24" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45404</v>
       </c>
@@ -2711,7 +2711,7 @@
       <c r="P24" s="9"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="19">
+      <c r="S24" s="16">
         <f t="shared" si="3"/>
         <v>45404</v>
       </c>
@@ -2726,7 +2726,7 @@
       <c r="X24" s="2"/>
     </row>
     <row r="25" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="19">
+      <c r="A25" s="16">
         <f t="shared" si="0"/>
         <v>45404</v>
       </c>
@@ -2745,7 +2745,7 @@
       <c r="F25" s="2">
         <v>54</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="16">
         <f t="shared" si="1"/>
         <v>45395</v>
       </c>
@@ -2758,7 +2758,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="19">
+      <c r="M25" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45405</v>
       </c>
@@ -2771,7 +2771,7 @@
       <c r="P25" s="9"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
-      <c r="S25" s="19">
+      <c r="S25" s="16">
         <f t="shared" si="3"/>
         <v>45405</v>
       </c>
@@ -2786,7 +2786,7 @@
       <c r="X25" s="2"/>
     </row>
     <row r="26" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="19">
+      <c r="A26" s="16">
         <f t="shared" si="0"/>
         <v>45405</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="F26" s="2">
         <v>9</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="16">
         <f t="shared" si="1"/>
         <v>45396</v>
       </c>
@@ -2818,7 +2818,7 @@
       <c r="J26" s="9"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="19">
+      <c r="M26" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45406</v>
       </c>
@@ -2831,7 +2831,7 @@
       <c r="P26" s="9"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
-      <c r="S26" s="19">
+      <c r="S26" s="16">
         <f t="shared" si="3"/>
         <v>45406</v>
       </c>
@@ -2846,7 +2846,7 @@
       <c r="X26" s="2"/>
     </row>
     <row r="27" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="19">
+      <c r="A27" s="16">
         <f t="shared" si="0"/>
         <v>45406</v>
       </c>
@@ -2863,7 +2863,7 @@
       <c r="F27" s="2">
         <v>11</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="16">
         <f t="shared" si="1"/>
         <v>45397</v>
       </c>
@@ -2876,7 +2876,7 @@
       <c r="J27" s="9"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="19">
+      <c r="M27" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45407</v>
       </c>
@@ -2889,7 +2889,7 @@
       <c r="P27" s="9"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
-      <c r="S27" s="19">
+      <c r="S27" s="16">
         <f t="shared" si="3"/>
         <v>45407</v>
       </c>
@@ -2904,7 +2904,7 @@
       <c r="X27" s="2"/>
     </row>
     <row r="28" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="19">
+      <c r="A28" s="16">
         <f t="shared" si="0"/>
         <v>45407</v>
       </c>
@@ -2921,7 +2921,7 @@
       <c r="F28" s="2">
         <v>28</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="16">
         <f t="shared" si="1"/>
         <v>45398</v>
       </c>
@@ -2934,7 +2934,7 @@
       <c r="J28" s="9"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="19">
+      <c r="M28" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45408</v>
       </c>
@@ -2947,7 +2947,7 @@
       <c r="P28" s="9"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
-      <c r="S28" s="19">
+      <c r="S28" s="16">
         <f t="shared" si="3"/>
         <v>45408</v>
       </c>
@@ -2962,7 +2962,7 @@
       <c r="X28" s="2"/>
     </row>
     <row r="29" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="19">
+      <c r="A29" s="16">
         <f t="shared" si="0"/>
         <v>45408</v>
       </c>
@@ -2979,7 +2979,7 @@
       <c r="F29" s="2">
         <v>11</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="16">
         <f t="shared" si="1"/>
         <v>45399</v>
       </c>
@@ -2992,7 +2992,7 @@
       <c r="J29" s="9"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="19">
+      <c r="M29" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45409</v>
       </c>
@@ -3005,7 +3005,7 @@
       <c r="P29" s="9"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
-      <c r="S29" s="19">
+      <c r="S29" s="16">
         <f t="shared" si="3"/>
         <v>45409</v>
       </c>
@@ -3020,7 +3020,7 @@
       <c r="X29" s="2"/>
     </row>
     <row r="30" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="19">
+      <c r="A30" s="16">
         <f t="shared" si="0"/>
         <v>45409</v>
       </c>
@@ -3037,7 +3037,7 @@
       <c r="F30" s="2">
         <v>14</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="16">
         <f t="shared" si="1"/>
         <v>45400</v>
       </c>
@@ -3050,7 +3050,7 @@
       <c r="J30" s="9"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="19">
+      <c r="M30" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45410</v>
       </c>
@@ -3063,7 +3063,7 @@
       <c r="P30" s="9"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="19">
+      <c r="S30" s="16">
         <f t="shared" si="3"/>
         <v>45410</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="X30" s="2"/>
     </row>
     <row r="31" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="19">
+      <c r="A31" s="16">
         <f t="shared" si="0"/>
         <v>45410</v>
       </c>
@@ -3095,7 +3095,7 @@
       <c r="F31" s="2">
         <v>41</v>
       </c>
-      <c r="G31" s="19">
+      <c r="G31" s="16">
         <f t="shared" si="1"/>
         <v>45401</v>
       </c>
@@ -3108,7 +3108,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="19">
+      <c r="M31" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45411</v>
       </c>
@@ -3121,7 +3121,7 @@
       <c r="P31" s="9"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
-      <c r="S31" s="19">
+      <c r="S31" s="16">
         <f t="shared" si="3"/>
         <v>45411</v>
       </c>
@@ -3136,7 +3136,7 @@
       <c r="X31" s="2"/>
     </row>
     <row r="32" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="19">
+      <c r="A32" s="16">
         <f t="shared" si="0"/>
         <v>45411</v>
       </c>
@@ -3153,7 +3153,7 @@
       <c r="F32" s="2">
         <v>19</v>
       </c>
-      <c r="G32" s="19">
+      <c r="G32" s="16">
         <f t="shared" si="1"/>
         <v>45402</v>
       </c>
@@ -3166,7 +3166,7 @@
       <c r="J32" s="9"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="19">
+      <c r="M32" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45412</v>
       </c>
@@ -3179,7 +3179,7 @@
       <c r="P32" s="9"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-      <c r="S32" s="19">
+      <c r="S32" s="16">
         <f t="shared" si="3"/>
         <v>45412</v>
       </c>
@@ -3194,7 +3194,7 @@
       <c r="X32" s="2"/>
     </row>
     <row r="33" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="19">
+      <c r="A33" s="16">
         <f t="shared" si="0"/>
         <v>45412</v>
       </c>
@@ -3213,7 +3213,7 @@
       <c r="F33" s="2">
         <v>37</v>
       </c>
-      <c r="G33" s="19">
+      <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>45403</v>
       </c>
@@ -3226,7 +3226,7 @@
       <c r="J33" s="9"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="19">
+      <c r="M33" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45413</v>
       </c>
@@ -3239,7 +3239,7 @@
       <c r="P33" s="9"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
-      <c r="S33" s="19">
+      <c r="S33" s="16">
         <f t="shared" si="3"/>
         <v>45413</v>
       </c>
@@ -3254,7 +3254,7 @@
       <c r="X33" s="2"/>
     </row>
     <row r="34" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="19">
+      <c r="A34" s="16">
         <f t="shared" si="0"/>
         <v>45413</v>
       </c>
@@ -3271,7 +3271,7 @@
       <c r="F34" s="2">
         <v>14</v>
       </c>
-      <c r="G34" s="19">
+      <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>45404</v>
       </c>
@@ -3284,7 +3284,7 @@
       <c r="J34" s="9"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
-      <c r="M34" s="19">
+      <c r="M34" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45414</v>
       </c>
@@ -3297,7 +3297,7 @@
       <c r="P34" s="9"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
-      <c r="S34" s="19">
+      <c r="S34" s="16">
         <f t="shared" si="3"/>
         <v>45414</v>
       </c>
@@ -3312,7 +3312,7 @@
       <c r="X34" s="2"/>
     </row>
     <row r="35" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="19">
+      <c r="A35" s="16">
         <f t="shared" si="0"/>
         <v>45414</v>
       </c>
@@ -3329,7 +3329,7 @@
       <c r="F35" s="2">
         <v>20</v>
       </c>
-      <c r="G35" s="19">
+      <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>45405</v>
       </c>
@@ -3342,7 +3342,7 @@
       <c r="J35" s="9"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
-      <c r="M35" s="19">
+      <c r="M35" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45415</v>
       </c>
@@ -3355,7 +3355,7 @@
       <c r="P35" s="9"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
-      <c r="S35" s="19">
+      <c r="S35" s="16">
         <f t="shared" si="3"/>
         <v>45415</v>
       </c>
@@ -3370,7 +3370,7 @@
       <c r="X35" s="2"/>
     </row>
     <row r="36" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="19">
+      <c r="A36" s="16">
         <f t="shared" si="0"/>
         <v>45415</v>
       </c>
@@ -3387,7 +3387,7 @@
       <c r="F36" s="2">
         <v>37</v>
       </c>
-      <c r="G36" s="19">
+      <c r="G36" s="16">
         <f t="shared" si="1"/>
         <v>45406</v>
       </c>
@@ -3400,7 +3400,7 @@
       <c r="J36" s="9"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="19">
+      <c r="M36" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45416</v>
       </c>
@@ -3413,7 +3413,7 @@
       <c r="P36" s="9"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
-      <c r="S36" s="19">
+      <c r="S36" s="16">
         <f t="shared" si="3"/>
         <v>45416</v>
       </c>
@@ -3428,7 +3428,7 @@
       <c r="X36" s="2"/>
     </row>
     <row r="37" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="19">
+      <c r="A37" s="16">
         <f t="shared" si="0"/>
         <v>45416</v>
       </c>
@@ -3445,7 +3445,7 @@
       <c r="F37" s="2">
         <v>24</v>
       </c>
-      <c r="G37" s="19">
+      <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>45407</v>
       </c>
@@ -3458,7 +3458,7 @@
       <c r="J37" s="9"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
-      <c r="M37" s="19">
+      <c r="M37" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45417</v>
       </c>
@@ -3471,7 +3471,7 @@
       <c r="P37" s="9"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
-      <c r="S37" s="19">
+      <c r="S37" s="16">
         <f t="shared" si="3"/>
         <v>45417</v>
       </c>
@@ -3486,7 +3486,7 @@
       <c r="X37" s="2"/>
     </row>
     <row r="38" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="19">
+      <c r="A38" s="16">
         <f t="shared" si="0"/>
         <v>45417</v>
       </c>
@@ -3503,7 +3503,7 @@
       <c r="F38" s="2">
         <v>5</v>
       </c>
-      <c r="G38" s="19">
+      <c r="G38" s="16">
         <f t="shared" si="1"/>
         <v>45408</v>
       </c>
@@ -3516,7 +3516,7 @@
       <c r="J38" s="9"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
-      <c r="M38" s="19">
+      <c r="M38" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45418</v>
       </c>
@@ -3529,7 +3529,7 @@
       <c r="P38" s="9"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
-      <c r="S38" s="19">
+      <c r="S38" s="16">
         <f t="shared" si="3"/>
         <v>45418</v>
       </c>
@@ -3544,7 +3544,7 @@
       <c r="X38" s="2"/>
     </row>
     <row r="39" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="19">
+      <c r="A39" s="16">
         <f t="shared" si="0"/>
         <v>45418</v>
       </c>
@@ -3561,7 +3561,7 @@
       <c r="F39" s="2">
         <v>16</v>
       </c>
-      <c r="G39" s="19">
+      <c r="G39" s="16">
         <f t="shared" si="1"/>
         <v>45409</v>
       </c>
@@ -3574,7 +3574,7 @@
       <c r="J39" s="9"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
-      <c r="M39" s="19">
+      <c r="M39" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45419</v>
       </c>
@@ -3587,7 +3587,7 @@
       <c r="P39" s="9"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
-      <c r="S39" s="19">
+      <c r="S39" s="16">
         <f t="shared" si="3"/>
         <v>45419</v>
       </c>
@@ -3602,7 +3602,7 @@
       <c r="X39" s="2"/>
     </row>
     <row r="40" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="19">
+      <c r="A40" s="16">
         <f t="shared" si="0"/>
         <v>45419</v>
       </c>
@@ -3619,7 +3619,7 @@
       <c r="F40" s="2">
         <v>58</v>
       </c>
-      <c r="G40" s="19">
+      <c r="G40" s="16">
         <f t="shared" si="1"/>
         <v>45410</v>
       </c>
@@ -3632,7 +3632,7 @@
       <c r="J40" s="9"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
-      <c r="M40" s="19">
+      <c r="M40" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45420</v>
       </c>
@@ -3645,7 +3645,7 @@
       <c r="P40" s="9"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
-      <c r="S40" s="19">
+      <c r="S40" s="16">
         <f t="shared" si="3"/>
         <v>45420</v>
       </c>
@@ -3660,7 +3660,7 @@
       <c r="X40" s="2"/>
     </row>
     <row r="41" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="19">
+      <c r="A41" s="16">
         <f t="shared" si="0"/>
         <v>45420</v>
       </c>
@@ -3673,7 +3673,7 @@
       <c r="D41" s="9"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="19">
+      <c r="G41" s="16">
         <f t="shared" si="1"/>
         <v>45411</v>
       </c>
@@ -3686,7 +3686,7 @@
       <c r="J41" s="9"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
-      <c r="M41" s="19">
+      <c r="M41" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45421</v>
       </c>
@@ -3699,7 +3699,7 @@
       <c r="P41" s="9"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
-      <c r="S41" s="19">
+      <c r="S41" s="16">
         <f t="shared" si="3"/>
         <v>45421</v>
       </c>
@@ -3714,7 +3714,7 @@
       <c r="X41" s="2"/>
     </row>
     <row r="42" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="19">
+      <c r="A42" s="16">
         <f t="shared" si="0"/>
         <v>45421</v>
       </c>
@@ -3727,7 +3727,7 @@
       <c r="D42" s="9"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="19">
+      <c r="G42" s="16">
         <f t="shared" si="1"/>
         <v>45412</v>
       </c>
@@ -3740,7 +3740,7 @@
       <c r="J42" s="9"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
-      <c r="M42" s="19">
+      <c r="M42" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45422</v>
       </c>
@@ -3753,7 +3753,7 @@
       <c r="P42" s="9"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
-      <c r="S42" s="19">
+      <c r="S42" s="16">
         <f t="shared" si="3"/>
         <v>45422</v>
       </c>
@@ -3768,7 +3768,7 @@
       <c r="X42" s="2"/>
     </row>
     <row r="43" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="19">
+      <c r="A43" s="16">
         <f t="shared" si="0"/>
         <v>45422</v>
       </c>
@@ -3781,7 +3781,7 @@
       <c r="D43" s="9"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="19">
+      <c r="G43" s="16">
         <f t="shared" si="1"/>
         <v>45413</v>
       </c>
@@ -3794,7 +3794,7 @@
       <c r="J43" s="9"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="19">
+      <c r="M43" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45423</v>
       </c>
@@ -3807,7 +3807,7 @@
       <c r="P43" s="9"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
-      <c r="S43" s="19">
+      <c r="S43" s="16">
         <f t="shared" si="3"/>
         <v>45423</v>
       </c>
@@ -3822,7 +3822,7 @@
       <c r="X43" s="2"/>
     </row>
     <row r="44" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="19">
+      <c r="A44" s="16">
         <f t="shared" si="0"/>
         <v>45423</v>
       </c>
@@ -3835,7 +3835,7 @@
       <c r="D44" s="9"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="19">
+      <c r="G44" s="16">
         <f t="shared" si="1"/>
         <v>45414</v>
       </c>
@@ -3848,7 +3848,7 @@
       <c r="J44" s="9"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="19">
+      <c r="M44" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45424</v>
       </c>
@@ -3861,7 +3861,7 @@
       <c r="P44" s="9"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
-      <c r="S44" s="19">
+      <c r="S44" s="16">
         <f t="shared" si="3"/>
         <v>45424</v>
       </c>
@@ -3876,7 +3876,7 @@
       <c r="X44" s="2"/>
     </row>
     <row r="45" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="19">
+      <c r="A45" s="16">
         <f t="shared" si="0"/>
         <v>45424</v>
       </c>
@@ -3889,7 +3889,7 @@
       <c r="D45" s="9"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="19">
+      <c r="G45" s="16">
         <f t="shared" si="1"/>
         <v>45415</v>
       </c>
@@ -3902,7 +3902,7 @@
       <c r="J45" s="9"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="19">
+      <c r="M45" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45425</v>
       </c>
@@ -3915,7 +3915,7 @@
       <c r="P45" s="9"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
-      <c r="S45" s="19">
+      <c r="S45" s="16">
         <f t="shared" si="3"/>
         <v>45425</v>
       </c>
@@ -3930,7 +3930,7 @@
       <c r="X45" s="2"/>
     </row>
     <row r="46" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="19">
+      <c r="A46" s="16">
         <f t="shared" si="0"/>
         <v>45425</v>
       </c>
@@ -3943,7 +3943,7 @@
       <c r="D46" s="9"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="19">
+      <c r="G46" s="16">
         <f t="shared" si="1"/>
         <v>45416</v>
       </c>
@@ -3956,7 +3956,7 @@
       <c r="J46" s="9"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
-      <c r="M46" s="19">
+      <c r="M46" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45426</v>
       </c>
@@ -3969,7 +3969,7 @@
       <c r="P46" s="9"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
-      <c r="S46" s="19">
+      <c r="S46" s="16">
         <f t="shared" si="3"/>
         <v>45426</v>
       </c>
@@ -3984,7 +3984,7 @@
       <c r="X46" s="2"/>
     </row>
     <row r="47" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="19">
+      <c r="A47" s="16">
         <f t="shared" si="0"/>
         <v>45426</v>
       </c>
@@ -3997,7 +3997,7 @@
       <c r="D47" s="9"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="19">
+      <c r="G47" s="16">
         <f t="shared" si="1"/>
         <v>45417</v>
       </c>
@@ -4010,7 +4010,7 @@
       <c r="J47" s="9"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
-      <c r="M47" s="19">
+      <c r="M47" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45427</v>
       </c>
@@ -4023,7 +4023,7 @@
       <c r="P47" s="9"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
-      <c r="S47" s="19">
+      <c r="S47" s="16">
         <f t="shared" si="3"/>
         <v>45427</v>
       </c>
@@ -4038,7 +4038,7 @@
       <c r="X47" s="2"/>
     </row>
     <row r="48" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="19">
+      <c r="A48" s="16">
         <f t="shared" si="0"/>
         <v>45427</v>
       </c>
@@ -4051,7 +4051,7 @@
       <c r="D48" s="9"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="19">
+      <c r="G48" s="16">
         <f t="shared" si="1"/>
         <v>45418</v>
       </c>
@@ -4064,7 +4064,7 @@
       <c r="J48" s="9"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
-      <c r="M48" s="19">
+      <c r="M48" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45428</v>
       </c>
@@ -4077,7 +4077,7 @@
       <c r="P48" s="9"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
-      <c r="S48" s="19">
+      <c r="S48" s="16">
         <f t="shared" si="3"/>
         <v>45428</v>
       </c>
@@ -4092,7 +4092,7 @@
       <c r="X48" s="2"/>
     </row>
     <row r="49" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="19">
+      <c r="A49" s="16">
         <f t="shared" si="0"/>
         <v>45428</v>
       </c>
@@ -4105,7 +4105,7 @@
       <c r="D49" s="9"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="19">
+      <c r="G49" s="16">
         <f t="shared" si="1"/>
         <v>45419</v>
       </c>
@@ -4118,7 +4118,7 @@
       <c r="J49" s="9"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
-      <c r="M49" s="19">
+      <c r="M49" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45429</v>
       </c>
@@ -4131,7 +4131,7 @@
       <c r="P49" s="9"/>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
-      <c r="S49" s="19">
+      <c r="S49" s="16">
         <f t="shared" si="3"/>
         <v>45429</v>
       </c>
@@ -4146,7 +4146,7 @@
       <c r="X49" s="2"/>
     </row>
     <row r="50" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="19">
+      <c r="A50" s="16">
         <f t="shared" si="0"/>
         <v>45429</v>
       </c>
@@ -4159,7 +4159,7 @@
       <c r="D50" s="9"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="19">
+      <c r="G50" s="16">
         <f t="shared" si="1"/>
         <v>45420</v>
       </c>
@@ -4172,7 +4172,7 @@
       <c r="J50" s="9"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
-      <c r="M50" s="19">
+      <c r="M50" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45430</v>
       </c>
@@ -4185,7 +4185,7 @@
       <c r="P50" s="9"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
-      <c r="S50" s="19">
+      <c r="S50" s="16">
         <f t="shared" si="3"/>
         <v>45430</v>
       </c>
@@ -4200,7 +4200,7 @@
       <c r="X50" s="2"/>
     </row>
     <row r="51" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="19">
+      <c r="A51" s="16">
         <f t="shared" si="0"/>
         <v>45430</v>
       </c>
@@ -4213,7 +4213,7 @@
       <c r="D51" s="9"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="19">
+      <c r="G51" s="16">
         <f t="shared" si="1"/>
         <v>45421</v>
       </c>
@@ -4226,7 +4226,7 @@
       <c r="J51" s="9"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
-      <c r="M51" s="19">
+      <c r="M51" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45431</v>
       </c>
@@ -4239,7 +4239,7 @@
       <c r="P51" s="9"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
-      <c r="S51" s="19">
+      <c r="S51" s="16">
         <f t="shared" si="3"/>
         <v>45431</v>
       </c>
@@ -4254,7 +4254,7 @@
       <c r="X51" s="2"/>
     </row>
     <row r="52" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="19">
+      <c r="A52" s="16">
         <f t="shared" si="0"/>
         <v>45431</v>
       </c>
@@ -4267,7 +4267,7 @@
       <c r="D52" s="9"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="19">
+      <c r="G52" s="16">
         <f t="shared" si="1"/>
         <v>45422</v>
       </c>
@@ -4280,7 +4280,7 @@
       <c r="J52" s="9"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
-      <c r="M52" s="19">
+      <c r="M52" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45432</v>
       </c>
@@ -4293,7 +4293,7 @@
       <c r="P52" s="9"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
-      <c r="S52" s="19">
+      <c r="S52" s="16">
         <f t="shared" si="3"/>
         <v>45432</v>
       </c>
@@ -4308,7 +4308,7 @@
       <c r="X52" s="2"/>
     </row>
     <row r="53" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="19">
+      <c r="A53" s="16">
         <f t="shared" si="0"/>
         <v>45432</v>
       </c>
@@ -4321,7 +4321,7 @@
       <c r="D53" s="9"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="19">
+      <c r="G53" s="16">
         <f t="shared" si="1"/>
         <v>45423</v>
       </c>
@@ -4334,7 +4334,7 @@
       <c r="J53" s="9"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
-      <c r="M53" s="19">
+      <c r="M53" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45433</v>
       </c>
@@ -4347,7 +4347,7 @@
       <c r="P53" s="9"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
-      <c r="S53" s="19">
+      <c r="S53" s="16">
         <f t="shared" si="3"/>
         <v>45433</v>
       </c>
@@ -4362,7 +4362,7 @@
       <c r="X53" s="2"/>
     </row>
     <row r="54" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="19">
+      <c r="A54" s="16">
         <f t="shared" si="0"/>
         <v>45433</v>
       </c>
@@ -4375,7 +4375,7 @@
       <c r="D54" s="9"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
-      <c r="G54" s="19">
+      <c r="G54" s="16">
         <f t="shared" si="1"/>
         <v>45424</v>
       </c>
@@ -4388,7 +4388,7 @@
       <c r="J54" s="9"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
-      <c r="M54" s="19">
+      <c r="M54" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45434</v>
       </c>
@@ -4401,7 +4401,7 @@
       <c r="P54" s="9"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
-      <c r="S54" s="19">
+      <c r="S54" s="16">
         <f t="shared" si="3"/>
         <v>45434</v>
       </c>
@@ -4416,7 +4416,7 @@
       <c r="X54" s="2"/>
     </row>
     <row r="55" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="19">
+      <c r="A55" s="16">
         <f t="shared" si="0"/>
         <v>45434</v>
       </c>
@@ -4429,7 +4429,7 @@
       <c r="D55" s="9"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-      <c r="G55" s="19">
+      <c r="G55" s="16">
         <f t="shared" si="1"/>
         <v>45425</v>
       </c>
@@ -4442,7 +4442,7 @@
       <c r="J55" s="9"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
-      <c r="M55" s="19">
+      <c r="M55" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45435</v>
       </c>
@@ -4455,7 +4455,7 @@
       <c r="P55" s="9"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
-      <c r="S55" s="19">
+      <c r="S55" s="16">
         <f t="shared" si="3"/>
         <v>45435</v>
       </c>
@@ -4470,7 +4470,7 @@
       <c r="X55" s="2"/>
     </row>
     <row r="56" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="19">
+      <c r="A56" s="16">
         <f t="shared" si="0"/>
         <v>45435</v>
       </c>
@@ -4483,7 +4483,7 @@
       <c r="D56" s="9"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="19">
+      <c r="G56" s="16">
         <f t="shared" si="1"/>
         <v>45426</v>
       </c>
@@ -4496,7 +4496,7 @@
       <c r="J56" s="9"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
-      <c r="M56" s="19">
+      <c r="M56" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45436</v>
       </c>
@@ -4509,7 +4509,7 @@
       <c r="P56" s="9"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
-      <c r="S56" s="19">
+      <c r="S56" s="16">
         <f t="shared" si="3"/>
         <v>45436</v>
       </c>
@@ -4524,7 +4524,7 @@
       <c r="X56" s="2"/>
     </row>
     <row r="57" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="19">
+      <c r="A57" s="16">
         <f t="shared" si="0"/>
         <v>45436</v>
       </c>
@@ -4537,7 +4537,7 @@
       <c r="D57" s="9"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
-      <c r="G57" s="19">
+      <c r="G57" s="16">
         <f t="shared" si="1"/>
         <v>45427</v>
       </c>
@@ -4550,7 +4550,7 @@
       <c r="J57" s="9"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
-      <c r="M57" s="19">
+      <c r="M57" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45437</v>
       </c>
@@ -4563,7 +4563,7 @@
       <c r="P57" s="9"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
-      <c r="S57" s="19">
+      <c r="S57" s="16">
         <f t="shared" si="3"/>
         <v>45437</v>
       </c>
@@ -4578,7 +4578,7 @@
       <c r="X57" s="2"/>
     </row>
     <row r="58" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="19">
+      <c r="A58" s="16">
         <f t="shared" si="0"/>
         <v>45437</v>
       </c>
@@ -4591,7 +4591,7 @@
       <c r="D58" s="9"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="19">
+      <c r="G58" s="16">
         <f t="shared" si="1"/>
         <v>45428</v>
       </c>
@@ -4604,7 +4604,7 @@
       <c r="J58" s="9"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
-      <c r="M58" s="19">
+      <c r="M58" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45438</v>
       </c>
@@ -4617,7 +4617,7 @@
       <c r="P58" s="9"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
-      <c r="S58" s="19">
+      <c r="S58" s="16">
         <f t="shared" si="3"/>
         <v>45438</v>
       </c>
@@ -4632,7 +4632,7 @@
       <c r="X58" s="2"/>
     </row>
     <row r="59" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="19">
+      <c r="A59" s="16">
         <f t="shared" si="0"/>
         <v>45438</v>
       </c>
@@ -4645,7 +4645,7 @@
       <c r="D59" s="9"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
-      <c r="G59" s="19">
+      <c r="G59" s="16">
         <f t="shared" si="1"/>
         <v>45429</v>
       </c>
@@ -4658,7 +4658,7 @@
       <c r="J59" s="9"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
-      <c r="M59" s="19">
+      <c r="M59" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45439</v>
       </c>
@@ -4671,7 +4671,7 @@
       <c r="P59" s="9"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
-      <c r="S59" s="19">
+      <c r="S59" s="16">
         <f t="shared" si="3"/>
         <v>45439</v>
       </c>
@@ -4686,7 +4686,7 @@
       <c r="X59" s="2"/>
     </row>
     <row r="60" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="19">
+      <c r="A60" s="16">
         <f t="shared" si="0"/>
         <v>45439</v>
       </c>
@@ -4699,7 +4699,7 @@
       <c r="D60" s="9"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
-      <c r="G60" s="19">
+      <c r="G60" s="16">
         <f t="shared" si="1"/>
         <v>45430</v>
       </c>
@@ -4712,7 +4712,7 @@
       <c r="J60" s="9"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
-      <c r="M60" s="19">
+      <c r="M60" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45440</v>
       </c>
@@ -4725,7 +4725,7 @@
       <c r="P60" s="9"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
-      <c r="S60" s="19">
+      <c r="S60" s="16">
         <f t="shared" si="3"/>
         <v>45440</v>
       </c>
@@ -4740,7 +4740,7 @@
       <c r="X60" s="2"/>
     </row>
     <row r="61" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="19">
+      <c r="A61" s="16">
         <f t="shared" si="0"/>
         <v>45440</v>
       </c>
@@ -4753,7 +4753,7 @@
       <c r="D61" s="9"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
-      <c r="G61" s="19">
+      <c r="G61" s="16">
         <f t="shared" si="1"/>
         <v>45431</v>
       </c>
@@ -4766,7 +4766,7 @@
       <c r="J61" s="9"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
-      <c r="M61" s="19">
+      <c r="M61" s="16">
         <f t="shared" ca="1" si="2"/>
         <v>45441</v>
       </c>
@@ -4779,7 +4779,7 @@
       <c r="P61" s="9"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
-      <c r="S61" s="19">
+      <c r="S61" s="16">
         <f t="shared" si="3"/>
         <v>45441</v>
       </c>
@@ -4794,7 +4794,7 @@
       <c r="X61" s="2"/>
     </row>
     <row r="62" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="19">
+      <c r="A62" s="16">
         <f t="shared" si="0"/>
         <v>45441</v>
       </c>
@@ -4807,7 +4807,7 @@
       <c r="D62" s="9"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
-      <c r="G62" s="19">
+      <c r="G62" s="16">
         <f t="shared" si="1"/>
         <v>45432</v>
       </c>
@@ -4820,7 +4820,7 @@
       <c r="J62" s="9"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
-      <c r="M62" s="19"/>
+      <c r="M62" s="16"/>
       <c r="N62" s="1">
         <v>0.14583333333333301</v>
       </c>
@@ -4830,7 +4830,7 @@
       <c r="P62" s="9"/>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
-      <c r="S62" s="19">
+      <c r="S62" s="16">
         <f t="shared" si="3"/>
         <v>45442</v>
       </c>
@@ -4845,7 +4845,7 @@
       <c r="X62" s="2"/>
     </row>
     <row r="63" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="19">
+      <c r="A63" s="16">
         <f t="shared" si="0"/>
         <v>45442</v>
       </c>
@@ -4858,7 +4858,7 @@
       <c r="D63" s="9"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
-      <c r="G63" s="19">
+      <c r="G63" s="16">
         <f t="shared" si="1"/>
         <v>45433</v>
       </c>
@@ -4871,7 +4871,7 @@
       <c r="J63" s="9"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
-      <c r="M63" s="19"/>
+      <c r="M63" s="16"/>
       <c r="N63" s="1">
         <v>0.15277777777777801</v>
       </c>
@@ -4881,7 +4881,7 @@
       <c r="P63" s="9"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
-      <c r="S63" s="19">
+      <c r="S63" s="16">
         <f t="shared" si="3"/>
         <v>45443</v>
       </c>
@@ -4896,7 +4896,7 @@
       <c r="X63" s="2"/>
     </row>
     <row r="64" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="19">
+      <c r="A64" s="16">
         <f t="shared" si="0"/>
         <v>45443</v>
       </c>
@@ -4909,7 +4909,7 @@
       <c r="D64" s="9"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-      <c r="G64" s="19">
+      <c r="G64" s="16">
         <f t="shared" si="1"/>
         <v>45434</v>
       </c>
@@ -4922,7 +4922,7 @@
       <c r="J64" s="9"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
-      <c r="M64" s="19"/>
+      <c r="M64" s="16"/>
       <c r="N64" s="1">
         <v>0.15972222222222199</v>
       </c>
@@ -4932,7 +4932,7 @@
       <c r="P64" s="9"/>
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
-      <c r="S64" s="19">
+      <c r="S64" s="16">
         <f t="shared" si="3"/>
         <v>45444</v>
       </c>
@@ -4947,7 +4947,7 @@
       <c r="X64" s="2"/>
     </row>
     <row r="65" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="19">
+      <c r="A65" s="16">
         <f t="shared" si="0"/>
         <v>45444</v>
       </c>
@@ -4960,7 +4960,7 @@
       <c r="D65" s="9"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="19">
+      <c r="G65" s="16">
         <f t="shared" si="1"/>
         <v>45435</v>
       </c>
@@ -4973,7 +4973,7 @@
       <c r="J65" s="9"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
-      <c r="M65" s="19"/>
+      <c r="M65" s="16"/>
       <c r="N65" s="1">
         <v>0.16666666666666699</v>
       </c>
@@ -4983,7 +4983,7 @@
       <c r="P65" s="9"/>
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
-      <c r="S65" s="19">
+      <c r="S65" s="16">
         <f t="shared" si="3"/>
         <v>45445</v>
       </c>
@@ -4998,7 +4998,7 @@
       <c r="X65" s="2"/>
     </row>
     <row r="66" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="19">
+      <c r="A66" s="16">
         <f t="shared" si="0"/>
         <v>45445</v>
       </c>
@@ -5011,7 +5011,7 @@
       <c r="D66" s="9"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
-      <c r="G66" s="19">
+      <c r="G66" s="16">
         <f t="shared" si="1"/>
         <v>45436</v>
       </c>
@@ -5024,7 +5024,7 @@
       <c r="J66" s="9"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
-      <c r="M66" s="19"/>
+      <c r="M66" s="16"/>
       <c r="N66" s="1">
         <v>0.17361111111111099</v>
       </c>
@@ -5034,7 +5034,7 @@
       <c r="P66" s="9"/>
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
-      <c r="S66" s="19">
+      <c r="S66" s="16">
         <f t="shared" si="3"/>
         <v>45446</v>
       </c>
@@ -5049,7 +5049,7 @@
       <c r="X66" s="2"/>
     </row>
     <row r="67" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="19">
+      <c r="A67" s="16">
         <f t="shared" si="0"/>
         <v>45446</v>
       </c>
@@ -5062,7 +5062,7 @@
       <c r="D67" s="9"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
-      <c r="G67" s="19">
+      <c r="G67" s="16">
         <f t="shared" si="1"/>
         <v>45437</v>
       </c>
@@ -5075,7 +5075,7 @@
       <c r="J67" s="9"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
-      <c r="M67" s="19"/>
+      <c r="M67" s="16"/>
       <c r="N67" s="1">
         <v>0.180555555555556</v>
       </c>
@@ -5085,7 +5085,7 @@
       <c r="P67" s="9"/>
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
-      <c r="S67" s="19">
+      <c r="S67" s="16">
         <f t="shared" si="3"/>
         <v>45447</v>
       </c>
@@ -5100,7 +5100,7 @@
       <c r="X67" s="2"/>
     </row>
     <row r="68" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="19">
+      <c r="A68" s="16">
         <f t="shared" si="0"/>
         <v>45447</v>
       </c>
@@ -5113,7 +5113,7 @@
       <c r="D68" s="9"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
-      <c r="G68" s="19">
+      <c r="G68" s="16">
         <f t="shared" si="1"/>
         <v>45438</v>
       </c>
@@ -5126,7 +5126,7 @@
       <c r="J68" s="9"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
-      <c r="M68" s="19"/>
+      <c r="M68" s="16"/>
       <c r="N68" s="1">
         <v>0.1875</v>
       </c>
@@ -5136,7 +5136,7 @@
       <c r="P68" s="9"/>
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
-      <c r="S68" s="19">
+      <c r="S68" s="16">
         <f t="shared" si="3"/>
         <v>45448</v>
       </c>
@@ -5151,7 +5151,7 @@
       <c r="X68" s="2"/>
     </row>
     <row r="69" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="19">
+      <c r="A69" s="16">
         <f t="shared" si="0"/>
         <v>45448</v>
       </c>
@@ -5164,7 +5164,7 @@
       <c r="D69" s="9"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
-      <c r="G69" s="19">
+      <c r="G69" s="16">
         <f t="shared" si="1"/>
         <v>45439</v>
       </c>
@@ -5177,7 +5177,7 @@
       <c r="J69" s="9"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
-      <c r="M69" s="19"/>
+      <c r="M69" s="16"/>
       <c r="N69" s="1">
         <v>0.194444444444445</v>
       </c>
@@ -5187,7 +5187,7 @@
       <c r="P69" s="9"/>
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
-      <c r="S69" s="19">
+      <c r="S69" s="16">
         <f t="shared" si="3"/>
         <v>45449</v>
       </c>
@@ -5202,7 +5202,7 @@
       <c r="X69" s="2"/>
     </row>
     <row r="70" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="19">
+      <c r="A70" s="16">
         <f t="shared" ref="A70:A71" si="4">A69+1</f>
         <v>45449</v>
       </c>
@@ -5215,7 +5215,7 @@
       <c r="D70" s="9"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
-      <c r="G70" s="19">
+      <c r="G70" s="16">
         <f t="shared" ref="G70:G71" si="5">G69+1</f>
         <v>45440</v>
       </c>
@@ -5228,7 +5228,7 @@
       <c r="J70" s="9"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
-      <c r="M70" s="19"/>
+      <c r="M70" s="16"/>
       <c r="N70" s="1">
         <v>0.20138888888888901</v>
       </c>
@@ -5238,7 +5238,7 @@
       <c r="P70" s="9"/>
       <c r="Q70" s="2"/>
       <c r="R70" s="2"/>
-      <c r="S70" s="19">
+      <c r="S70" s="16">
         <f t="shared" ref="S70:S71" si="6">S69+1</f>
         <v>45450</v>
       </c>
@@ -5253,7 +5253,7 @@
       <c r="X70" s="2"/>
     </row>
     <row r="71" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="19">
+      <c r="A71" s="16">
         <f t="shared" si="4"/>
         <v>45450</v>
       </c>
@@ -5266,7 +5266,7 @@
       <c r="D71" s="9"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="19">
+      <c r="G71" s="16">
         <f t="shared" si="5"/>
         <v>45441</v>
       </c>
@@ -5279,7 +5279,7 @@
       <c r="J71" s="9"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
-      <c r="M71" s="19"/>
+      <c r="M71" s="16"/>
       <c r="N71" s="1">
         <v>0.20833333333333301</v>
       </c>
@@ -5289,7 +5289,7 @@
       <c r="P71" s="9"/>
       <c r="Q71" s="2"/>
       <c r="R71" s="2"/>
-      <c r="S71" s="19">
+      <c r="S71" s="16">
         <f t="shared" si="6"/>
         <v>45451</v>
       </c>

</xml_diff>